<commit_message>
new spreadseet added in LinearProgramming.xlsx
</commit_message>
<xml_diff>
--- a/LinearProgramming.xlsx
+++ b/LinearProgramming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diele\OneDrive\Área de Trabalho\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D4C032-7B84-46CA-8C12-792B2B9DB333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D4525D-CD15-45DA-995F-CDA83316FA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{B20FA0A7-6B8D-4DE0-807A-25B715AF2B76}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{B20FA0A7-6B8D-4DE0-807A-25B715AF2B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Campanha eleitoral" sheetId="1" r:id="rId1"/>
@@ -18,186 +18,232 @@
     <sheet name="PC Tech" sheetId="4" r:id="rId3"/>
     <sheet name="Exercício - Tectona" sheetId="5" r:id="rId4"/>
     <sheet name="Corretora" sheetId="6" r:id="rId5"/>
+    <sheet name="exercício - ração" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Campanha eleitoral'!$A$1</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Campanha eleitoral'!$F$4,'Campanha eleitoral'!$E$4</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">Corretora!$E$4:$I$4</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">'exercício - ração'!$E$9:$G$9</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'Exercício - Tectona'!$J$4:$K$4</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'PC Tech'!$G$3,'PC Tech'!$H$3</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">Sheet2!$B$4,Sheet2!$C$4</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Campanha eleitoral'!$E$15</definedName>
     <definedName name="solver_lhs1" localSheetId="4" hidden="1">Corretora!$J$9</definedName>
+    <definedName name="solver_lhs1" localSheetId="5" hidden="1">'exercício - ração'!$F$18</definedName>
     <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Exercício - Tectona'!$E$13</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">'PC Tech'!$F$18</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sheet2!$D$13</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Campanha eleitoral'!$E$16</definedName>
     <definedName name="solver_lhs2" localSheetId="4" hidden="1">Corretora!$J$10</definedName>
+    <definedName name="solver_lhs2" localSheetId="5" hidden="1">'exercício - ração'!$F$19</definedName>
     <definedName name="solver_lhs2" localSheetId="3" hidden="1">'Exercício - Tectona'!$E$12</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">'PC Tech'!$F$19</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sheet2!$D$14</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Campanha eleitoral'!$E$17</definedName>
     <definedName name="solver_lhs3" localSheetId="4" hidden="1">Corretora!$J$11</definedName>
+    <definedName name="solver_lhs3" localSheetId="5" hidden="1">'exercício - ração'!$F$20</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">'PC Tech'!$F$20</definedName>
     <definedName name="solver_lhs4" localSheetId="4" hidden="1">Corretora!$J$12</definedName>
+    <definedName name="solver_lhs4" localSheetId="5" hidden="1">'exercício - ração'!$F$21</definedName>
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">'PC Tech'!$F$21</definedName>
+    <definedName name="solver_lhs5" localSheetId="5" hidden="1">'exercício - ração'!$F$22</definedName>
+    <definedName name="solver_lhs6" localSheetId="5" hidden="1">'exercício - ração'!$F$23</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="5" hidden="1">6</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Campanha eleitoral'!$B$6</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">Corretora!$B$7</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">'exercício - ração'!$F$14</definedName>
     <definedName name="solver_opt" localSheetId="3" hidden="1">'Exercício - Tectona'!$C$2</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">'PC Tech'!$G$9</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Sheet2!$B$9</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Campanha eleitoral'!$G$15</definedName>
     <definedName name="solver_rhs1" localSheetId="4" hidden="1">Corretora!$M$9</definedName>
+    <definedName name="solver_rhs1" localSheetId="5" hidden="1">'exercício - ração'!$H$18</definedName>
     <definedName name="solver_rhs1" localSheetId="3" hidden="1">'Exercício - Tectona'!$G$13</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">'PC Tech'!$H$18</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">Sheet2!$F$13</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Campanha eleitoral'!$G$16</definedName>
     <definedName name="solver_rhs2" localSheetId="4" hidden="1">Corretora!$M$10</definedName>
+    <definedName name="solver_rhs2" localSheetId="5" hidden="1">'exercício - ração'!$H$19</definedName>
     <definedName name="solver_rhs2" localSheetId="3" hidden="1">'Exercício - Tectona'!$G$12</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">'PC Tech'!$H$19</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">Sheet2!$F$14</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Campanha eleitoral'!$G$17</definedName>
     <definedName name="solver_rhs3" localSheetId="4" hidden="1">Corretora!$M$11</definedName>
+    <definedName name="solver_rhs3" localSheetId="5" hidden="1">'exercício - ração'!$H$20</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">'PC Tech'!$H$20</definedName>
     <definedName name="solver_rhs4" localSheetId="4" hidden="1">Corretora!$M$12</definedName>
+    <definedName name="solver_rhs4" localSheetId="5" hidden="1">'exercício - ração'!$H$21</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">'PC Tech'!$H$21</definedName>
+    <definedName name="solver_rhs5" localSheetId="5" hidden="1">'exercício - ração'!$H$22</definedName>
+    <definedName name="solver_rhs6" localSheetId="5" hidden="1">'exercício - ração'!$H$23</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
@@ -223,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="136">
   <si>
     <t>Função objeto:</t>
   </si>
@@ -581,20 +627,117 @@
   <si>
     <t>50.000 em Títulos municipais, 175.000 na Palmeer Technologies e 25.000 em ações de alto risco.</t>
   </si>
+  <si>
+    <t>min o custo</t>
+  </si>
+  <si>
+    <t>Exigência de dieta (ingredientes)</t>
+  </si>
+  <si>
+    <t>Produto de aveia (unidades/lb)</t>
+  </si>
+  <si>
+    <t>Grãos enriquecidos (unidades/lb)</t>
+  </si>
+  <si>
+    <t>Produto mineral (unidades/lb)</t>
+  </si>
+  <si>
+    <t>Necessidade diária mínima (unidades)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Custo/lb</t>
+  </si>
+  <si>
+    <t>F. objeto:</t>
+  </si>
+  <si>
+    <t>Quant. Max:</t>
+  </si>
+  <si>
+    <t>A+G+M &lt;= 2,5 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; = </t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>Tabela Nutricional</t>
+  </si>
+  <si>
+    <t>Quant. Max</t>
+  </si>
+  <si>
+    <t>Min A</t>
+  </si>
+  <si>
+    <t>Min E</t>
+  </si>
+  <si>
+    <t>Min D</t>
+  </si>
+  <si>
+    <t>Min B</t>
+  </si>
+  <si>
+    <t>Min C</t>
+  </si>
+  <si>
+    <t>xA+yG+zM &gt;= 5</t>
+  </si>
+  <si>
+    <t>xA+yG+zM &gt;= 2</t>
+  </si>
+  <si>
+    <t>xA+yG+zM &gt;= 10</t>
+  </si>
+  <si>
+    <t>xA+yG+zM &gt;= 7</t>
+  </si>
+  <si>
+    <t>xA+yG+zM &gt;= 6</t>
+  </si>
+  <si>
+    <t>Custo diário</t>
+  </si>
+  <si>
+    <t>lb por dia</t>
+  </si>
+  <si>
+    <t>0,25 lb de produto de aveia e 4,5 lb de grãos enriquecidos.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.0_ ;_-[$$-409]* \-#,##0.0\ ;_-[$$-409]* &quot;-&quot;?_ ;_-@_ "/>
+    <numFmt numFmtId="177" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -703,8 +846,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Var(--cds-font-family-source-sa"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -790,8 +944,25 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="47">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1395,8 +1566,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -1411,8 +1669,11 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1590,99 +1851,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="8" borderId="14" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1748,15 +1916,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1771,6 +1930,108 @@
     <xf numFmtId="164" fontId="1" fillId="14" borderId="16" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1780,15 +2041,119 @@
     <xf numFmtId="0" fontId="14" fillId="14" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="9" borderId="31" xfId="9" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="19" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="19" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="12" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="47" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="48" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="49" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="50" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="12" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="14" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="39" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="40" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="27" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="28" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="29" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="40" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="15" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="2" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="38" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="51" xfId="15" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="52" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="17" borderId="53" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="16" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="17">
     <cellStyle name="20% - Accent1" xfId="13" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="4" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="15" builtinId="50"/>
     <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="10" builtinId="39"/>
     <cellStyle name="60% - Accent2" xfId="6" builtinId="36"/>
+    <cellStyle name="60% - Accent6" xfId="16" builtinId="52"/>
     <cellStyle name="Accent1" xfId="12" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Accent6" xfId="14" builtinId="49"/>
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="9" builtinId="23"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2211,31 +2576,31 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="1"/>
-      <c r="L1" s="93" t="s">
+      <c r="L1" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="94"/>
-      <c r="S1" s="95"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="123"/>
+      <c r="P1" s="123"/>
+      <c r="Q1" s="123"/>
+      <c r="R1" s="123"/>
+      <c r="S1" s="124"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1">
-      <c r="D2" s="90" t="s">
+      <c r="D2" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="91"/>
-      <c r="F2" s="92"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="97"/>
-      <c r="S2" s="98"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="121"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="126"/>
+      <c r="N2" s="126"/>
+      <c r="O2" s="126"/>
+      <c r="P2" s="126"/>
+      <c r="Q2" s="126"/>
+      <c r="R2" s="126"/>
+      <c r="S2" s="127"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
@@ -2253,14 +2618,14 @@
       <c r="F3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="96"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="98"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="127"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
@@ -2278,14 +2643,14 @@
       <c r="F4" s="27">
         <v>10.000000000000007</v>
       </c>
-      <c r="L4" s="96"/>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="97"/>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="98"/>
+      <c r="L4" s="125"/>
+      <c r="M4" s="126"/>
+      <c r="N4" s="126"/>
+      <c r="O4" s="126"/>
+      <c r="P4" s="126"/>
+      <c r="Q4" s="126"/>
+      <c r="R4" s="126"/>
+      <c r="S4" s="127"/>
     </row>
     <row r="5" spans="1:19">
       <c r="D5" s="36" t="s">
@@ -2297,14 +2662,14 @@
       <c r="F5" s="29">
         <v>500</v>
       </c>
-      <c r="L5" s="96"/>
-      <c r="M5" s="97"/>
-      <c r="N5" s="97"/>
-      <c r="O5" s="97"/>
-      <c r="P5" s="97"/>
-      <c r="Q5" s="97"/>
-      <c r="R5" s="97"/>
-      <c r="S5" s="98"/>
+      <c r="L5" s="125"/>
+      <c r="M5" s="126"/>
+      <c r="N5" s="126"/>
+      <c r="O5" s="126"/>
+      <c r="P5" s="126"/>
+      <c r="Q5" s="126"/>
+      <c r="R5" s="126"/>
+      <c r="S5" s="127"/>
     </row>
     <row r="6" spans="1:19" ht="15" thickBot="1">
       <c r="A6" s="11" t="s">
@@ -2327,94 +2692,94 @@
       <c r="F6" s="30">
         <v>7000</v>
       </c>
-      <c r="L6" s="96"/>
-      <c r="M6" s="97"/>
-      <c r="N6" s="97"/>
-      <c r="O6" s="97"/>
-      <c r="P6" s="97"/>
-      <c r="Q6" s="97"/>
-      <c r="R6" s="97"/>
-      <c r="S6" s="98"/>
+      <c r="L6" s="125"/>
+      <c r="M6" s="126"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="126"/>
+      <c r="P6" s="126"/>
+      <c r="Q6" s="126"/>
+      <c r="R6" s="126"/>
+      <c r="S6" s="127"/>
     </row>
     <row r="7" spans="1:19">
       <c r="C7" s="4"/>
-      <c r="L7" s="96"/>
-      <c r="M7" s="97"/>
-      <c r="N7" s="97"/>
-      <c r="O7" s="97"/>
-      <c r="P7" s="97"/>
-      <c r="Q7" s="97"/>
-      <c r="R7" s="97"/>
-      <c r="S7" s="98"/>
+      <c r="L7" s="125"/>
+      <c r="M7" s="126"/>
+      <c r="N7" s="126"/>
+      <c r="O7" s="126"/>
+      <c r="P7" s="126"/>
+      <c r="Q7" s="126"/>
+      <c r="R7" s="126"/>
+      <c r="S7" s="127"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="L8" s="96"/>
-      <c r="M8" s="97"/>
-      <c r="N8" s="97"/>
-      <c r="O8" s="97"/>
-      <c r="P8" s="97"/>
-      <c r="Q8" s="97"/>
-      <c r="R8" s="97"/>
-      <c r="S8" s="98"/>
+      <c r="L8" s="125"/>
+      <c r="M8" s="126"/>
+      <c r="N8" s="126"/>
+      <c r="O8" s="126"/>
+      <c r="P8" s="126"/>
+      <c r="Q8" s="126"/>
+      <c r="R8" s="126"/>
+      <c r="S8" s="127"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="L9" s="96"/>
-      <c r="M9" s="97"/>
-      <c r="N9" s="97"/>
-      <c r="O9" s="97"/>
-      <c r="P9" s="97"/>
-      <c r="Q9" s="97"/>
-      <c r="R9" s="97"/>
-      <c r="S9" s="98"/>
+      <c r="L9" s="125"/>
+      <c r="M9" s="126"/>
+      <c r="N9" s="126"/>
+      <c r="O9" s="126"/>
+      <c r="P9" s="126"/>
+      <c r="Q9" s="126"/>
+      <c r="R9" s="126"/>
+      <c r="S9" s="127"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="L10" s="96"/>
-      <c r="M10" s="97"/>
-      <c r="N10" s="97"/>
-      <c r="O10" s="97"/>
-      <c r="P10" s="97"/>
-      <c r="Q10" s="97"/>
-      <c r="R10" s="97"/>
-      <c r="S10" s="98"/>
+      <c r="L10" s="125"/>
+      <c r="M10" s="126"/>
+      <c r="N10" s="126"/>
+      <c r="O10" s="126"/>
+      <c r="P10" s="126"/>
+      <c r="Q10" s="126"/>
+      <c r="R10" s="126"/>
+      <c r="S10" s="127"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="L11" s="96"/>
-      <c r="M11" s="97"/>
-      <c r="N11" s="97"/>
-      <c r="O11" s="97"/>
-      <c r="P11" s="97"/>
-      <c r="Q11" s="97"/>
-      <c r="R11" s="97"/>
-      <c r="S11" s="98"/>
+      <c r="L11" s="125"/>
+      <c r="M11" s="126"/>
+      <c r="N11" s="126"/>
+      <c r="O11" s="126"/>
+      <c r="P11" s="126"/>
+      <c r="Q11" s="126"/>
+      <c r="R11" s="126"/>
+      <c r="S11" s="127"/>
     </row>
     <row r="12" spans="1:19">
-      <c r="L12" s="96"/>
-      <c r="M12" s="97"/>
-      <c r="N12" s="97"/>
-      <c r="O12" s="97"/>
-      <c r="P12" s="97"/>
-      <c r="Q12" s="97"/>
-      <c r="R12" s="97"/>
-      <c r="S12" s="98"/>
+      <c r="L12" s="125"/>
+      <c r="M12" s="126"/>
+      <c r="N12" s="126"/>
+      <c r="O12" s="126"/>
+      <c r="P12" s="126"/>
+      <c r="Q12" s="126"/>
+      <c r="R12" s="126"/>
+      <c r="S12" s="127"/>
     </row>
     <row r="13" spans="1:19" ht="15" thickBot="1">
-      <c r="A13" s="87" t="s">
+      <c r="A13" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="89"/>
-      <c r="L13" s="99"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="100"/>
-      <c r="O13" s="100"/>
-      <c r="P13" s="100"/>
-      <c r="Q13" s="100"/>
-      <c r="R13" s="100"/>
-      <c r="S13" s="101"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="118"/>
+      <c r="L13" s="128"/>
+      <c r="M13" s="129"/>
+      <c r="N13" s="129"/>
+      <c r="O13" s="129"/>
+      <c r="P13" s="129"/>
+      <c r="Q13" s="129"/>
+      <c r="R13" s="129"/>
+      <c r="S13" s="130"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="14" t="s">
@@ -2531,10 +2896,10 @@
       <c r="B20" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="85" t="s">
+      <c r="C20" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="86"/>
+      <c r="D20" s="115"/>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1">
       <c r="B21" s="12" t="s">
@@ -2585,11 +2950,11 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1"/>
     <row r="2" spans="1:6" ht="15" thickBot="1">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="92"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="121"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="18" t="s">
@@ -2720,10 +3085,10 @@
       <c r="A17" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="85" t="s">
+      <c r="B17" s="114" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="86"/>
+      <c r="C17" s="115"/>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1">
       <c r="A18" s="12" t="s">
@@ -2767,16 +3132,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1">
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="119" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="92"/>
-      <c r="F1" s="105" t="s">
+      <c r="C1" s="120"/>
+      <c r="D1" s="121"/>
+      <c r="F1" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="106"/>
-      <c r="H1" s="107"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="136"/>
     </row>
     <row r="2" spans="2:9">
       <c r="B2" s="68"/>
@@ -2827,11 +3192,11 @@
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1"/>
     <row r="6" spans="2:9" ht="15" thickBot="1">
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="139" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="111"/>
-      <c r="D6" s="112"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="141"/>
       <c r="F6" s="1"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -2915,10 +3280,10 @@
       <c r="F11" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="108" t="s">
+      <c r="G11" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="109"/>
+      <c r="H11" s="138"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1">
       <c r="B12" s="63" t="s">
@@ -2975,15 +3340,15 @@
     </row>
     <row r="15" spans="2:9" ht="15" thickBot="1"/>
     <row r="16" spans="2:9" ht="15" thickBot="1">
-      <c r="B16" s="102" t="s">
+      <c r="B16" s="131" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="103"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="103"/>
-      <c r="F16" s="103"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="104"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="132"/>
+      <c r="G16" s="132"/>
+      <c r="H16" s="133"/>
     </row>
     <row r="17" spans="2:9">
       <c r="B17" s="56" t="s">
@@ -3174,11 +3539,11 @@
         <f ca="1">_xlfn.FORMULATEXT(C2)</f>
         <v>=SUMPRODUCT(J4:K4;E8:F8)</v>
       </c>
-      <c r="I2" s="113" t="s">
+      <c r="I2" s="142" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="114"/>
-      <c r="K2" s="115"/>
+      <c r="J2" s="143"/>
+      <c r="K2" s="144"/>
     </row>
     <row r="3" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="I3" s="79"/>
@@ -3236,10 +3601,10 @@
       <c r="I6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="108" t="s">
+      <c r="J6" s="137" t="s">
         <v>85</v>
       </c>
-      <c r="K6" s="109"/>
+      <c r="K6" s="138"/>
     </row>
     <row r="7" spans="1:11" ht="15" thickBot="1">
       <c r="D7" s="63" t="s">
@@ -3273,15 +3638,15 @@
     </row>
     <row r="9" spans="1:11" ht="15" thickBot="1"/>
     <row r="10" spans="1:11" ht="15" thickBot="1">
-      <c r="A10" s="102" t="s">
+      <c r="A10" s="131" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="103"/>
-      <c r="F10" s="103"/>
-      <c r="G10" s="104"/>
+      <c r="B10" s="132"/>
+      <c r="C10" s="132"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="133"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="56" t="s">
@@ -3382,8 +3747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{785D99A5-81F0-42C9-90F2-9FF2F905B0E4}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3406,169 +3771,169 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14" ht="21.6" thickBot="1">
-      <c r="D2" s="140" t="s">
+      <c r="D2" s="145" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="141"/>
-      <c r="F2" s="141"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="142"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="147"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="D3" s="135"/>
-      <c r="E3" s="133" t="s">
+      <c r="D3" s="104"/>
+      <c r="E3" s="102" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="133" t="s">
+      <c r="F3" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="133" t="s">
+      <c r="G3" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="133" t="s">
+      <c r="H3" s="102" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="134" t="s">
+      <c r="I3" s="103" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="143" t="s">
+      <c r="A4" s="109" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="144">
+      <c r="B4" s="110">
         <v>250000</v>
       </c>
-      <c r="D4" s="136" t="s">
+      <c r="D4" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="116">
+      <c r="E4" s="85">
         <v>50000</v>
       </c>
-      <c r="F4" s="116">
+      <c r="F4" s="85">
         <v>0</v>
       </c>
-      <c r="G4" s="116">
+      <c r="G4" s="85">
         <v>0</v>
       </c>
-      <c r="H4" s="116">
+      <c r="H4" s="85">
         <v>175000</v>
       </c>
-      <c r="I4" s="117">
+      <c r="I4" s="86">
         <v>25000</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1">
-      <c r="A5" s="143" t="s">
+      <c r="A5" s="109" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="137" t="s">
+      <c r="D5" s="106" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="118">
+      <c r="E5" s="87">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="F5" s="118">
+      <c r="F5" s="87">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="G5" s="118">
+      <c r="G5" s="87">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="H5" s="118">
+      <c r="H5" s="87">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="I5" s="119">
+      <c r="I5" s="88">
         <v>0.11799999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1"/>
     <row r="7" spans="1:14" ht="22.2" thickTop="1" thickBot="1">
-      <c r="A7" s="139" t="s">
+      <c r="A7" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="145">
+      <c r="B7" s="111">
         <f>SUMPRODUCT(E4:I4,E5:I5)</f>
         <v>20300</v>
       </c>
-      <c r="D7" s="140" t="s">
+      <c r="D7" s="145" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="141"/>
-      <c r="F7" s="141"/>
-      <c r="G7" s="141"/>
-      <c r="H7" s="141"/>
-      <c r="I7" s="141"/>
-      <c r="J7" s="141"/>
-      <c r="K7" s="141"/>
-      <c r="L7" s="141"/>
-      <c r="M7" s="142"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="146"/>
+      <c r="H7" s="146"/>
+      <c r="I7" s="146"/>
+      <c r="J7" s="146"/>
+      <c r="K7" s="146"/>
+      <c r="L7" s="146"/>
+      <c r="M7" s="147"/>
     </row>
     <row r="8" spans="1:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="D8" s="129" t="s">
+      <c r="D8" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="130" t="s">
+      <c r="E8" s="99" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="130" t="s">
+      <c r="F8" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="130" t="s">
+      <c r="G8" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="H8" s="130" t="s">
+      <c r="H8" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="130" t="s">
+      <c r="I8" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="J8" s="131" t="s">
+      <c r="J8" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="K8" s="131" t="s">
+      <c r="K8" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="131" t="s">
+      <c r="L8" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="M8" s="132" t="s">
+      <c r="M8" s="101" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="D9" s="138" t="s">
+      <c r="D9" s="107" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="125">
+      <c r="E9" s="94">
         <v>1</v>
       </c>
-      <c r="F9" s="125">
+      <c r="F9" s="94">
         <v>0</v>
       </c>
-      <c r="G9" s="125">
+      <c r="G9" s="94">
         <v>0</v>
       </c>
-      <c r="H9" s="125">
+      <c r="H9" s="94">
         <v>0</v>
       </c>
-      <c r="I9" s="125">
+      <c r="I9" s="94">
         <v>0</v>
       </c>
-      <c r="J9" s="126">
+      <c r="J9" s="95">
         <f>SUMPRODUCT($E$4:$I$4,E9:I9)</f>
         <v>50000</v>
       </c>
       <c r="K9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="127">
+      <c r="L9" s="96">
         <v>0.2</v>
       </c>
-      <c r="M9" s="128">
+      <c r="M9" s="97">
         <f>L9*$B$4</f>
         <v>50000</v>
       </c>
@@ -3578,7 +3943,7 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="D10" s="136" t="s">
+      <c r="D10" s="105" t="s">
         <v>97</v>
       </c>
       <c r="E10" s="6">
@@ -3603,7 +3968,7 @@
       <c r="K10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="120">
+      <c r="L10" s="89">
         <v>0.4</v>
       </c>
       <c r="M10" s="29">
@@ -3616,7 +3981,7 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="D11" s="136" t="s">
+      <c r="D11" s="105" t="s">
         <v>98</v>
       </c>
       <c r="E11" s="6">
@@ -3641,7 +4006,7 @@
       <c r="K11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="120">
+      <c r="L11" s="89">
         <v>0.5</v>
       </c>
       <c r="M11" s="29">
@@ -3654,35 +4019,35 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1">
-      <c r="D12" s="137" t="s">
+      <c r="D12" s="106" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="121">
+      <c r="E12" s="90">
         <v>1</v>
       </c>
-      <c r="F12" s="121">
+      <c r="F12" s="90">
         <v>1</v>
       </c>
-      <c r="G12" s="121">
+      <c r="G12" s="90">
         <v>1</v>
       </c>
-      <c r="H12" s="121">
+      <c r="H12" s="90">
         <v>1</v>
       </c>
-      <c r="I12" s="121">
+      <c r="I12" s="90">
         <v>1</v>
       </c>
-      <c r="J12" s="122">
+      <c r="J12" s="91">
         <f>SUMPRODUCT($E$4:$I$4,E12:I12)</f>
         <v>250000</v>
       </c>
       <c r="K12" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="L12" s="123">
+      <c r="L12" s="92">
         <v>1</v>
       </c>
-      <c r="M12" s="124">
+      <c r="M12" s="93">
         <f>L12*B4</f>
         <v>250000</v>
       </c>
@@ -3693,7 +4058,7 @@
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1"/>
     <row r="16" spans="1:14" ht="15" thickBot="1">
-      <c r="E16" s="146" t="s">
+      <c r="E16" s="112" t="s">
         <v>35</v>
       </c>
       <c r="F16" s="148" t="s">
@@ -3704,10 +4069,10 @@
       <c r="I16" s="150"/>
     </row>
     <row r="17" spans="5:6" ht="15" thickBot="1">
-      <c r="E17" s="146" t="s">
+      <c r="E17" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="147">
+      <c r="F17" s="113">
         <f>B7</f>
         <v>20300</v>
       </c>
@@ -3720,4 +4085,385 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFCEFA5-DCA8-40BA-B334-969A07003C5E}">
+  <dimension ref="D1:I27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:8" ht="20.399999999999999" thickBot="1">
+      <c r="D1" s="168" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="170"/>
+    </row>
+    <row r="2" spans="4:8" ht="15" thickBot="1">
+      <c r="D2" s="164" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="165" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="166" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="166" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="167" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="4:8">
+      <c r="D3" s="154" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="156">
+        <v>3</v>
+      </c>
+      <c r="F3" s="157">
+        <v>4</v>
+      </c>
+      <c r="G3" s="157">
+        <v>2</v>
+      </c>
+      <c r="H3" s="158">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="4:8">
+      <c r="D4" s="154" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="159">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="151">
+        <v>1</v>
+      </c>
+      <c r="G4" s="151">
+        <v>1</v>
+      </c>
+      <c r="H4" s="160">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8">
+      <c r="D5" s="154" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="159">
+        <v>4</v>
+      </c>
+      <c r="F5" s="151">
+        <v>2</v>
+      </c>
+      <c r="G5" s="151">
+        <v>6</v>
+      </c>
+      <c r="H5" s="160">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8">
+      <c r="D6" s="154" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="159">
+        <v>1</v>
+      </c>
+      <c r="F6" s="151">
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="151">
+        <v>2</v>
+      </c>
+      <c r="H6" s="160">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8">
+      <c r="D7" s="154" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="159">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="151">
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="151">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="160">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8">
+      <c r="D8" s="154" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="161">
+        <v>0.09</v>
+      </c>
+      <c r="F8" s="152">
+        <v>0.12</v>
+      </c>
+      <c r="G8" s="152">
+        <v>0.18</v>
+      </c>
+      <c r="H8" s="160"/>
+    </row>
+    <row r="9" spans="4:8" ht="15" thickBot="1">
+      <c r="D9" s="155" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="162">
+        <v>0.25</v>
+      </c>
+      <c r="F9" s="163">
+        <v>4.4999999999999991</v>
+      </c>
+      <c r="G9" s="163">
+        <v>0</v>
+      </c>
+      <c r="H9" s="30"/>
+    </row>
+    <row r="12" spans="4:8">
+      <c r="E12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" ht="15" thickBot="1">
+      <c r="E13" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="3">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" ht="15.6" thickTop="1" thickBot="1">
+      <c r="E14" s="171" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" s="153">
+        <f>SUMPRODUCT(E8:G8,E9:G9)</f>
+        <v>0.56249999999999989</v>
+      </c>
+      <c r="G14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" ht="15" thickTop="1"/>
+    <row r="16" spans="4:8" ht="15" thickBot="1"/>
+    <row r="17" spans="4:9" ht="15" thickBot="1">
+      <c r="D17" s="172" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="173" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="178" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="178" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="179" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9">
+      <c r="D18" s="174" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="17">
+        <f>SUM(E9:G9)</f>
+        <v>4.7499999999999991</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="32">
+        <f>F13</f>
+        <v>6</v>
+      </c>
+      <c r="I18" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(F18)</f>
+        <v>=SUM(E9:G9)</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9">
+      <c r="D19" s="175" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="177" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" s="7">
+        <f>SUMPRODUCT(E3:G3,$E$9:$G$9)</f>
+        <v>18.749999999999996</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="H19" s="52">
+        <f>H3</f>
+        <v>5</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" ref="I19:I23" ca="1" si="0">_xlfn.FORMULATEXT(F19)</f>
+        <v>=SUMPRODUCT(E3:G3;$E$9:$G$9)</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9">
+      <c r="D20" s="175" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="177" t="s">
+        <v>129</v>
+      </c>
+      <c r="F20" s="7">
+        <f>SUMPRODUCT(E4:G4,$E$9:$G$9)</f>
+        <v>4.6249999999999991</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="52">
+        <f>H4</f>
+        <v>2</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SUMPRODUCT(E4:G4;$E$9:$G$9)</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9">
+      <c r="D21" s="175" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" s="177" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="7">
+        <f>SUMPRODUCT(E5:G5,$E$9:$G$9)</f>
+        <v>9.9999999999999982</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="52">
+        <f>H5</f>
+        <v>10</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SUMPRODUCT(E5:G5;$E$9:$G$9)</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9">
+      <c r="D22" s="175" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" s="177" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" s="7">
+        <f>SUMPRODUCT(E6:G6,$E$9:$G$9)</f>
+        <v>6.9999999999999982</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="52">
+        <f>H6</f>
+        <v>7</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SUMPRODUCT(E6:G6;$E$9:$G$9)</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" ht="15" thickBot="1">
+      <c r="D23" s="176" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23" s="54">
+        <f>SUMPRODUCT(E7:G7,$E$9:$G$9)</f>
+        <v>6.8749999999999982</v>
+      </c>
+      <c r="G23" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="30">
+        <f>H7</f>
+        <v>6</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SUMPRODUCT(E7:G7;$E$9:$G$9)</v>
+      </c>
+    </row>
+    <row r="25" spans="4:9" ht="15" thickBot="1"/>
+    <row r="26" spans="4:9" ht="15" thickBot="1">
+      <c r="E26" s="180" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="183" t="s">
+        <v>135</v>
+      </c>
+      <c r="G26" s="181"/>
+    </row>
+    <row r="27" spans="4:9" ht="15" thickBot="1">
+      <c r="E27" s="185" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="184">
+        <f>F14</f>
+        <v>0.56249999999999989</v>
+      </c>
+      <c r="G27" s="182" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="F26:G26"/>
+  </mergeCells>
+  <phoneticPr fontId="16" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Transportation Problem added and README updated
</commit_message>
<xml_diff>
--- a/LinearProgramming.xlsx
+++ b/LinearProgramming.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diele\OneDrive\Área de Trabalho\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diele\OneDrive\Área de Trabalho\Excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8355B784-58A8-47B0-BFBE-8250E9798BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B189ED-BA24-4C51-BC11-4310B065526A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="8" xr2:uid="{B20FA0A7-6B8D-4DE0-807A-25B715AF2B76}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="7" xr2:uid="{B20FA0A7-6B8D-4DE0-807A-25B715AF2B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Campanha eleitoral" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="High School" sheetId="8" r:id="rId7"/>
     <sheet name="exercício - ônibus" sheetId="9" r:id="rId8"/>
     <sheet name="Nike Factory" sheetId="10" r:id="rId9"/>
+    <sheet name="Transportation problem" sheetId="11" r:id="rId10"/>
+    <sheet name="Transportation problem 2" sheetId="12" r:id="rId11"/>
+    <sheet name="TP - Exercise" sheetId="13" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Campanha eleitoral'!$A$1</definedName>
@@ -33,6 +36,9 @@
     <definedName name="solver_adj" localSheetId="8" hidden="1">'Nike Factory'!$F$6:$G$6</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'PC Tech'!$G$3,'PC Tech'!$H$3</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">Sheet2!$B$4,Sheet2!$C$4</definedName>
+    <definedName name="solver_adj" localSheetId="11" hidden="1">'TP - Exercise'!$B$12:$D$14</definedName>
+    <definedName name="solver_adj" localSheetId="9" hidden="1">'Transportation problem'!$C$11:$E$13</definedName>
+    <definedName name="solver_adj" localSheetId="10" hidden="1">'Transportation problem 2'!$D$4:$D$12</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
@@ -41,6 +47,9 @@
     <definedName name="solver_cvg" localSheetId="8" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="11" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="9" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="10" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
@@ -49,6 +58,9 @@
     <definedName name="solver_drv" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="9" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="10" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="5" hidden="1">2</definedName>
@@ -57,6 +69,9 @@
     <definedName name="solver_eng" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="9" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
@@ -65,6 +80,9 @@
     <definedName name="solver_est" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="9" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="10" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
@@ -73,6 +91,9 @@
     <definedName name="solver_itr" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="9" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="10" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Campanha eleitoral'!$E$15</definedName>
     <definedName name="solver_lhs1" localSheetId="4" hidden="1">Corretora!$J$9</definedName>
     <definedName name="solver_lhs1" localSheetId="5" hidden="1">'exercício - ração'!$F$18</definedName>
@@ -81,6 +102,9 @@
     <definedName name="solver_lhs1" localSheetId="8" hidden="1">'Nike Factory'!$F$11</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">'PC Tech'!$F$18</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sheet2!$D$13</definedName>
+    <definedName name="solver_lhs1" localSheetId="11" hidden="1">'TP - Exercise'!$B$15:$D$15</definedName>
+    <definedName name="solver_lhs1" localSheetId="9" hidden="1">'Transportation problem'!$C$14:$E$14</definedName>
+    <definedName name="solver_lhs1" localSheetId="10" hidden="1">'Transportation problem 2'!$B$16:$B$18</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Campanha eleitoral'!$E$16</definedName>
     <definedName name="solver_lhs2" localSheetId="4" hidden="1">Corretora!$J$10</definedName>
     <definedName name="solver_lhs2" localSheetId="5" hidden="1">'exercício - ração'!$F$19</definedName>
@@ -89,6 +113,9 @@
     <definedName name="solver_lhs2" localSheetId="8" hidden="1">'Nike Factory'!$F$12</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">'PC Tech'!$F$19</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sheet2!$D$14</definedName>
+    <definedName name="solver_lhs2" localSheetId="11" hidden="1">'TP - Exercise'!$E$12:$E$14</definedName>
+    <definedName name="solver_lhs2" localSheetId="9" hidden="1">'Transportation problem'!$F$11:$F$13</definedName>
+    <definedName name="solver_lhs2" localSheetId="10" hidden="1">'Transportation problem 2'!$B$22:$B$24</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Campanha eleitoral'!$E$17</definedName>
     <definedName name="solver_lhs3" localSheetId="4" hidden="1">Corretora!$J$11</definedName>
     <definedName name="solver_lhs3" localSheetId="5" hidden="1">'exercício - ração'!$F$20</definedName>
@@ -112,6 +139,9 @@
     <definedName name="solver_mip" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="9" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="10" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
@@ -120,6 +150,9 @@
     <definedName name="solver_mni" localSheetId="8" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="11" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="9" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="10" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
@@ -128,6 +161,9 @@
     <definedName name="solver_mrt" localSheetId="8" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="11" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="9" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="10" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
@@ -136,6 +172,9 @@
     <definedName name="solver_msl" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="9" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
@@ -144,6 +183,9 @@
     <definedName name="solver_neg" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="9" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="10" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
@@ -152,6 +194,9 @@
     <definedName name="solver_nod" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="9" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="10" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="5" hidden="1">6</definedName>
@@ -160,6 +205,9 @@
     <definedName name="solver_num" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="9" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
@@ -168,6 +216,9 @@
     <definedName name="solver_nwt" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="9" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="10" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Campanha eleitoral'!$B$6</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">Corretora!$B$7</definedName>
     <definedName name="solver_opt" localSheetId="5" hidden="1">'exercício - ração'!$F$14</definedName>
@@ -176,6 +227,9 @@
     <definedName name="solver_opt" localSheetId="8" hidden="1">'Nike Factory'!$J$7</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">'PC Tech'!$G$9</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Sheet2!$B$9</definedName>
+    <definedName name="solver_opt" localSheetId="11" hidden="1">'TP - Exercise'!$H$8</definedName>
+    <definedName name="solver_opt" localSheetId="9" hidden="1">'Transportation problem'!$I$9</definedName>
+    <definedName name="solver_opt" localSheetId="10" hidden="1">'Transportation problem 2'!$H$7</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
@@ -184,6 +238,9 @@
     <definedName name="solver_pre" localSheetId="8" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="11" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="9" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="10" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
@@ -192,6 +249,9 @@
     <definedName name="solver_rbv" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="9" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="10" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="5" hidden="1">1</definedName>
@@ -200,6 +260,9 @@
     <definedName name="solver_rel1" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="11" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="9" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="10" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="5" hidden="1">3</definedName>
@@ -208,6 +271,9 @@
     <definedName name="solver_rel2" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="9" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="5" hidden="1">3</definedName>
@@ -231,6 +297,9 @@
     <definedName name="solver_rhs1" localSheetId="8" hidden="1">'Nike Factory'!$H$11</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">'PC Tech'!$H$18</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">Sheet2!$F$13</definedName>
+    <definedName name="solver_rhs1" localSheetId="11" hidden="1">'TP - Exercise'!$B$8:$D$8</definedName>
+    <definedName name="solver_rhs1" localSheetId="9" hidden="1">'Transportation problem'!$C$7:$E$7</definedName>
+    <definedName name="solver_rhs1" localSheetId="10" hidden="1">'Transportation problem 2'!$D$16:$D$18</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Campanha eleitoral'!$G$16</definedName>
     <definedName name="solver_rhs2" localSheetId="4" hidden="1">Corretora!$M$10</definedName>
     <definedName name="solver_rhs2" localSheetId="5" hidden="1">'exercício - ração'!$H$19</definedName>
@@ -239,6 +308,9 @@
     <definedName name="solver_rhs2" localSheetId="8" hidden="1">'Nike Factory'!$H$12</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">'PC Tech'!$H$19</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">Sheet2!$F$14</definedName>
+    <definedName name="solver_rhs2" localSheetId="11" hidden="1">'TP - Exercise'!$E$5:$E$7</definedName>
+    <definedName name="solver_rhs2" localSheetId="9" hidden="1">'Transportation problem'!$F$4:$F$6</definedName>
+    <definedName name="solver_rhs2" localSheetId="10" hidden="1">'Transportation problem 2'!$D$22:$D$24</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Campanha eleitoral'!$G$17</definedName>
     <definedName name="solver_rhs3" localSheetId="4" hidden="1">Corretora!$M$11</definedName>
     <definedName name="solver_rhs3" localSheetId="5" hidden="1">'exercício - ração'!$H$20</definedName>
@@ -262,6 +334,9 @@
     <definedName name="solver_rlx" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="9" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
@@ -270,6 +345,9 @@
     <definedName name="solver_rsd" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="11" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="9" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="10" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
@@ -278,6 +356,9 @@
     <definedName name="solver_scl" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="9" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="10" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
@@ -286,6 +367,9 @@
     <definedName name="solver_sho" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="9" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
@@ -294,6 +378,9 @@
     <definedName name="solver_ssz" localSheetId="8" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="11" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="9" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="10" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
@@ -302,6 +389,9 @@
     <definedName name="solver_tim" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="9" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="10" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
@@ -310,6 +400,9 @@
     <definedName name="solver_tol" localSheetId="8" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="11" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="9" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="10" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="5" hidden="1">2</definedName>
@@ -318,6 +411,9 @@
     <definedName name="solver_typ" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="9" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
@@ -326,6 +422,9 @@
     <definedName name="solver_val" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="11" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="9" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="10" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
@@ -334,6 +433,9 @@
     <definedName name="solver_ver" localSheetId="8" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="11" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="9" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="10" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -356,7 +458,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="246">
   <si>
     <t>Função objeto:</t>
   </si>
@@ -1026,6 +1128,120 @@
   <si>
     <t>Total Profit</t>
   </si>
+  <si>
+    <t>Data table:</t>
+  </si>
+  <si>
+    <t>Albany</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>Des Moines</t>
+  </si>
+  <si>
+    <t>Evanston</t>
+  </si>
+  <si>
+    <t>Ft Lauderdale</t>
+  </si>
+  <si>
+    <t>Demanda</t>
+  </si>
+  <si>
+    <t>Fábrica</t>
+  </si>
+  <si>
+    <t>Loja</t>
+  </si>
+  <si>
+    <t>Envios:</t>
+  </si>
+  <si>
+    <t>Tot produzido</t>
+  </si>
+  <si>
+    <t>Tot enviado</t>
+  </si>
+  <si>
+    <t>Custo Total:</t>
+  </si>
+  <si>
+    <t>Factories</t>
+  </si>
+  <si>
+    <t>Unit Costs</t>
+  </si>
+  <si>
+    <t>Shipments</t>
+  </si>
+  <si>
+    <t>Stores</t>
+  </si>
+  <si>
+    <t>Suply Constraints</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Capacidade</t>
+  </si>
+  <si>
+    <t>Demand Constraints</t>
+  </si>
+  <si>
+    <t>Inflow</t>
+  </si>
+  <si>
+    <t>Outflow</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Transportation Problem - Template 1</t>
+  </si>
+  <si>
+    <t>Custos de envio por caminhão de concreto</t>
+  </si>
+  <si>
+    <t>Capacidade de envio</t>
+  </si>
+  <si>
+    <t>Filial 1</t>
+  </si>
+  <si>
+    <t>Filial 2</t>
+  </si>
+  <si>
+    <t>Filial 3</t>
+  </si>
+  <si>
+    <t>Projeto A</t>
+  </si>
+  <si>
+    <t>Projeto B</t>
+  </si>
+  <si>
+    <t>Projeto C</t>
+  </si>
+  <si>
+    <t>Total enviado</t>
+  </si>
+  <si>
+    <t>Total recebido</t>
+  </si>
+  <si>
+    <t>Transportation Problem</t>
+  </si>
+  <si>
+    <t>Envios</t>
+  </si>
 </sst>
 </file>
 
@@ -1040,7 +1256,7 @@
     <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.0_ ;_-[$$-409]* \-#,##0.0\ ;_-[$$-409]* &quot;-&quot;?_ ;_-@_ "/>
     <numFmt numFmtId="169" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1182,8 +1398,16 @@
       <color rgb="FF1F1F1F"/>
       <name val="Var(--cds-font-family-source-sa"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1292,8 +1516,13 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="58">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -2032,8 +2261,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -2054,8 +2298,10 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="54" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="58" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="282">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2398,136 +2644,10 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="16" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="12" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="12" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="52" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="38" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2614,12 +2734,6 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="2" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="52" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="38" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="16" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2659,15 +2773,6 @@
     <xf numFmtId="0" fontId="19" fillId="12" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2685,10 +2790,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2696,7 +2797,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="9" borderId="31" xfId="9" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="18" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2723,12 +2823,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="36" xfId="17" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="17" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="33" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2748,6 +2842,184 @@
     <xf numFmtId="164" fontId="1" fillId="17" borderId="16" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="58" xfId="20" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="12" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="12" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="52" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="38" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="52" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="38" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="36" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="11" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2757,8 +3029,27 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="13" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="54" xfId="17" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="21" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="22">
     <cellStyle name="20% - Accent1" xfId="13" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="4" builtinId="34"/>
     <cellStyle name="20% - Accent6" xfId="15" builtinId="50"/>
@@ -2769,6 +3060,7 @@
     <cellStyle name="60% - Accent6" xfId="16" builtinId="52"/>
     <cellStyle name="Accent1" xfId="12" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Accent4" xfId="21" builtinId="41"/>
     <cellStyle name="Accent6" xfId="14" builtinId="49"/>
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="9" builtinId="23"/>
@@ -2778,6 +3070,7 @@
     <cellStyle name="Heading 4" xfId="18" builtinId="19"/>
     <cellStyle name="Input" xfId="8" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="20" builtinId="21"/>
     <cellStyle name="Percent" xfId="11" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3194,31 +3487,31 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="1"/>
-      <c r="L1" s="152" t="s">
+      <c r="L1" s="231" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="153"/>
-      <c r="N1" s="153"/>
-      <c r="O1" s="153"/>
-      <c r="P1" s="153"/>
-      <c r="Q1" s="153"/>
-      <c r="R1" s="153"/>
-      <c r="S1" s="154"/>
+      <c r="M1" s="232"/>
+      <c r="N1" s="232"/>
+      <c r="O1" s="232"/>
+      <c r="P1" s="232"/>
+      <c r="Q1" s="232"/>
+      <c r="R1" s="232"/>
+      <c r="S1" s="233"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1">
-      <c r="D2" s="149" t="s">
+      <c r="D2" s="228" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="150"/>
-      <c r="F2" s="151"/>
-      <c r="L2" s="155"/>
-      <c r="M2" s="156"/>
-      <c r="N2" s="156"/>
-      <c r="O2" s="156"/>
-      <c r="P2" s="156"/>
-      <c r="Q2" s="156"/>
-      <c r="R2" s="156"/>
-      <c r="S2" s="157"/>
+      <c r="E2" s="229"/>
+      <c r="F2" s="230"/>
+      <c r="L2" s="234"/>
+      <c r="M2" s="235"/>
+      <c r="N2" s="235"/>
+      <c r="O2" s="235"/>
+      <c r="P2" s="235"/>
+      <c r="Q2" s="235"/>
+      <c r="R2" s="235"/>
+      <c r="S2" s="236"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
@@ -3236,14 +3529,14 @@
       <c r="F3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="155"/>
-      <c r="M3" s="156"/>
-      <c r="N3" s="156"/>
-      <c r="O3" s="156"/>
-      <c r="P3" s="156"/>
-      <c r="Q3" s="156"/>
-      <c r="R3" s="156"/>
-      <c r="S3" s="157"/>
+      <c r="L3" s="234"/>
+      <c r="M3" s="235"/>
+      <c r="N3" s="235"/>
+      <c r="O3" s="235"/>
+      <c r="P3" s="235"/>
+      <c r="Q3" s="235"/>
+      <c r="R3" s="235"/>
+      <c r="S3" s="236"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
@@ -3261,14 +3554,14 @@
       <c r="F4" s="27">
         <v>10.000000000000007</v>
       </c>
-      <c r="L4" s="155"/>
-      <c r="M4" s="156"/>
-      <c r="N4" s="156"/>
-      <c r="O4" s="156"/>
-      <c r="P4" s="156"/>
-      <c r="Q4" s="156"/>
-      <c r="R4" s="156"/>
-      <c r="S4" s="157"/>
+      <c r="L4" s="234"/>
+      <c r="M4" s="235"/>
+      <c r="N4" s="235"/>
+      <c r="O4" s="235"/>
+      <c r="P4" s="235"/>
+      <c r="Q4" s="235"/>
+      <c r="R4" s="235"/>
+      <c r="S4" s="236"/>
     </row>
     <row r="5" spans="1:19">
       <c r="D5" s="36" t="s">
@@ -3280,14 +3573,14 @@
       <c r="F5" s="29">
         <v>500</v>
       </c>
-      <c r="L5" s="155"/>
-      <c r="M5" s="156"/>
-      <c r="N5" s="156"/>
-      <c r="O5" s="156"/>
-      <c r="P5" s="156"/>
-      <c r="Q5" s="156"/>
-      <c r="R5" s="156"/>
-      <c r="S5" s="157"/>
+      <c r="L5" s="234"/>
+      <c r="M5" s="235"/>
+      <c r="N5" s="235"/>
+      <c r="O5" s="235"/>
+      <c r="P5" s="235"/>
+      <c r="Q5" s="235"/>
+      <c r="R5" s="235"/>
+      <c r="S5" s="236"/>
     </row>
     <row r="6" spans="1:19" ht="15" thickBot="1">
       <c r="A6" s="11" t="s">
@@ -3310,94 +3603,94 @@
       <c r="F6" s="30">
         <v>7000</v>
       </c>
-      <c r="L6" s="155"/>
-      <c r="M6" s="156"/>
-      <c r="N6" s="156"/>
-      <c r="O6" s="156"/>
-      <c r="P6" s="156"/>
-      <c r="Q6" s="156"/>
-      <c r="R6" s="156"/>
-      <c r="S6" s="157"/>
+      <c r="L6" s="234"/>
+      <c r="M6" s="235"/>
+      <c r="N6" s="235"/>
+      <c r="O6" s="235"/>
+      <c r="P6" s="235"/>
+      <c r="Q6" s="235"/>
+      <c r="R6" s="235"/>
+      <c r="S6" s="236"/>
     </row>
     <row r="7" spans="1:19">
       <c r="C7" s="4"/>
-      <c r="L7" s="155"/>
-      <c r="M7" s="156"/>
-      <c r="N7" s="156"/>
-      <c r="O7" s="156"/>
-      <c r="P7" s="156"/>
-      <c r="Q7" s="156"/>
-      <c r="R7" s="156"/>
-      <c r="S7" s="157"/>
+      <c r="L7" s="234"/>
+      <c r="M7" s="235"/>
+      <c r="N7" s="235"/>
+      <c r="O7" s="235"/>
+      <c r="P7" s="235"/>
+      <c r="Q7" s="235"/>
+      <c r="R7" s="235"/>
+      <c r="S7" s="236"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="L8" s="155"/>
-      <c r="M8" s="156"/>
-      <c r="N8" s="156"/>
-      <c r="O8" s="156"/>
-      <c r="P8" s="156"/>
-      <c r="Q8" s="156"/>
-      <c r="R8" s="156"/>
-      <c r="S8" s="157"/>
+      <c r="L8" s="234"/>
+      <c r="M8" s="235"/>
+      <c r="N8" s="235"/>
+      <c r="O8" s="235"/>
+      <c r="P8" s="235"/>
+      <c r="Q8" s="235"/>
+      <c r="R8" s="235"/>
+      <c r="S8" s="236"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="L9" s="155"/>
-      <c r="M9" s="156"/>
-      <c r="N9" s="156"/>
-      <c r="O9" s="156"/>
-      <c r="P9" s="156"/>
-      <c r="Q9" s="156"/>
-      <c r="R9" s="156"/>
-      <c r="S9" s="157"/>
+      <c r="L9" s="234"/>
+      <c r="M9" s="235"/>
+      <c r="N9" s="235"/>
+      <c r="O9" s="235"/>
+      <c r="P9" s="235"/>
+      <c r="Q9" s="235"/>
+      <c r="R9" s="235"/>
+      <c r="S9" s="236"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="L10" s="155"/>
-      <c r="M10" s="156"/>
-      <c r="N10" s="156"/>
-      <c r="O10" s="156"/>
-      <c r="P10" s="156"/>
-      <c r="Q10" s="156"/>
-      <c r="R10" s="156"/>
-      <c r="S10" s="157"/>
+      <c r="L10" s="234"/>
+      <c r="M10" s="235"/>
+      <c r="N10" s="235"/>
+      <c r="O10" s="235"/>
+      <c r="P10" s="235"/>
+      <c r="Q10" s="235"/>
+      <c r="R10" s="235"/>
+      <c r="S10" s="236"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="L11" s="155"/>
-      <c r="M11" s="156"/>
-      <c r="N11" s="156"/>
-      <c r="O11" s="156"/>
-      <c r="P11" s="156"/>
-      <c r="Q11" s="156"/>
-      <c r="R11" s="156"/>
-      <c r="S11" s="157"/>
+      <c r="L11" s="234"/>
+      <c r="M11" s="235"/>
+      <c r="N11" s="235"/>
+      <c r="O11" s="235"/>
+      <c r="P11" s="235"/>
+      <c r="Q11" s="235"/>
+      <c r="R11" s="235"/>
+      <c r="S11" s="236"/>
     </row>
     <row r="12" spans="1:19">
-      <c r="L12" s="155"/>
-      <c r="M12" s="156"/>
-      <c r="N12" s="156"/>
-      <c r="O12" s="156"/>
-      <c r="P12" s="156"/>
-      <c r="Q12" s="156"/>
-      <c r="R12" s="156"/>
-      <c r="S12" s="157"/>
+      <c r="L12" s="234"/>
+      <c r="M12" s="235"/>
+      <c r="N12" s="235"/>
+      <c r="O12" s="235"/>
+      <c r="P12" s="235"/>
+      <c r="Q12" s="235"/>
+      <c r="R12" s="235"/>
+      <c r="S12" s="236"/>
     </row>
     <row r="13" spans="1:19" ht="15" thickBot="1">
-      <c r="A13" s="146" t="s">
+      <c r="A13" s="225" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="147"/>
-      <c r="C13" s="147"/>
-      <c r="D13" s="147"/>
-      <c r="E13" s="147"/>
-      <c r="F13" s="147"/>
-      <c r="G13" s="148"/>
-      <c r="L13" s="158"/>
-      <c r="M13" s="159"/>
-      <c r="N13" s="159"/>
-      <c r="O13" s="159"/>
-      <c r="P13" s="159"/>
-      <c r="Q13" s="159"/>
-      <c r="R13" s="159"/>
-      <c r="S13" s="160"/>
+      <c r="B13" s="226"/>
+      <c r="C13" s="226"/>
+      <c r="D13" s="226"/>
+      <c r="E13" s="226"/>
+      <c r="F13" s="226"/>
+      <c r="G13" s="227"/>
+      <c r="L13" s="237"/>
+      <c r="M13" s="238"/>
+      <c r="N13" s="238"/>
+      <c r="O13" s="238"/>
+      <c r="P13" s="238"/>
+      <c r="Q13" s="238"/>
+      <c r="R13" s="238"/>
+      <c r="S13" s="239"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="14" t="s">
@@ -3514,10 +3807,10 @@
       <c r="B20" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="144" t="s">
+      <c r="C20" s="223" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="145"/>
+      <c r="D20" s="224"/>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1">
       <c r="B21" s="12" t="s">
@@ -3552,6 +3845,855 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C315B69-61BD-4FBA-9669-1B9A14C74D2C}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="277" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="277"/>
+      <c r="C1" s="277"/>
+      <c r="D1" s="277"/>
+      <c r="E1" s="277"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="277"/>
+      <c r="H1" s="277"/>
+      <c r="I1" s="277"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" thickBot="1">
+      <c r="A2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="276" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="276"/>
+      <c r="D2" s="276"/>
+      <c r="E2" s="276"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="212"/>
+      <c r="C3" s="213" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="213" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="83" t="s">
+        <v>211</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="275" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4" s="214" t="s">
+        <v>212</v>
+      </c>
+      <c r="C4" s="9">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9">
+        <v>4</v>
+      </c>
+      <c r="E4" s="29">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="275"/>
+      <c r="B5" s="214" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" s="9">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9">
+        <v>4</v>
+      </c>
+      <c r="E5" s="29">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" thickBot="1">
+      <c r="A6" s="275"/>
+      <c r="B6" s="215" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" s="91">
+        <v>9</v>
+      </c>
+      <c r="D6" s="91">
+        <v>7</v>
+      </c>
+      <c r="E6" s="93">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="B7" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" s="3">
+        <v>300</v>
+      </c>
+      <c r="D7" s="3">
+        <v>200</v>
+      </c>
+      <c r="E7" s="3">
+        <v>200</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="15" thickBot="1">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="H9" t="s">
+        <v>221</v>
+      </c>
+      <c r="I9" s="217">
+        <f>SUMPRODUCT(C11:E13,C4:E6)</f>
+        <v>3900</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" ref="L9" ca="1" si="0">_xlfn.FORMULATEXT(I9)</f>
+        <v>=SUMPRODUCT(C11:E13;C4:E6)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" s="212"/>
+      <c r="C10" s="213" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="213" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" s="83" t="s">
+        <v>211</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="275" t="s">
+        <v>216</v>
+      </c>
+      <c r="B11" s="214" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" s="216">
+        <v>100</v>
+      </c>
+      <c r="D11" s="216">
+        <v>0</v>
+      </c>
+      <c r="E11" s="216">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <f>SUM(C11:E11)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="275"/>
+      <c r="B12" s="214" t="s">
+        <v>213</v>
+      </c>
+      <c r="C12" s="216">
+        <v>0</v>
+      </c>
+      <c r="D12" s="216">
+        <v>200</v>
+      </c>
+      <c r="E12" s="216">
+        <v>100</v>
+      </c>
+      <c r="F12" s="3">
+        <f>SUM(C12:E12)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" thickBot="1">
+      <c r="A13" s="275"/>
+      <c r="B13" s="215" t="s">
+        <v>214</v>
+      </c>
+      <c r="C13" s="216">
+        <v>200</v>
+      </c>
+      <c r="D13" s="216">
+        <v>0</v>
+      </c>
+      <c r="E13" s="216">
+        <v>100</v>
+      </c>
+      <c r="F13" s="3">
+        <f>SUM(C13:E13)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="B14" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C14" s="3">
+        <f>SUM(C11:C13)</f>
+        <v>300</v>
+      </c>
+      <c r="D14" s="3">
+        <f>SUM(D11:D13)</f>
+        <v>200</v>
+      </c>
+      <c r="E14" s="3">
+        <f>SUM(E11:E13)</f>
+        <v>200</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F527DF-9B05-49FA-AD76-7A3E3BEA9005}">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="278" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="278"/>
+      <c r="C1" s="278"/>
+      <c r="D1" s="278"/>
+      <c r="E1" s="278"/>
+      <c r="F1" s="278"/>
+      <c r="G1" s="278"/>
+      <c r="H1" s="278"/>
+      <c r="I1" s="278"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="147" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="147" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" s="147" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" s="147" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="147" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="9">
+        <v>5</v>
+      </c>
+      <c r="D4" s="148">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="147" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" s="9">
+        <v>4</v>
+      </c>
+      <c r="D5" s="148">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="147" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="9">
+        <v>3</v>
+      </c>
+      <c r="D6" s="148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="147" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" s="9">
+        <v>8</v>
+      </c>
+      <c r="D7" s="148">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>221</v>
+      </c>
+      <c r="H7" s="217">
+        <f>SUMPRODUCT(C4:C12,D4:D12)</f>
+        <v>3900</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" ref="K7" ca="1" si="0">_xlfn.FORMULATEXT(H7)</f>
+        <v>=SUMPRODUCT(C4:C12;D4:D12)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="147" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" s="9">
+        <v>4</v>
+      </c>
+      <c r="D8" s="148">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="147" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="148">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="147" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C10" s="9">
+        <v>9</v>
+      </c>
+      <c r="D10" s="148">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="147" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" s="9">
+        <v>7</v>
+      </c>
+      <c r="D11" s="148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="147" t="s">
+        <v>214</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C12" s="9">
+        <v>5</v>
+      </c>
+      <c r="D12" s="148">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="147" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="147" t="s">
+        <v>231</v>
+      </c>
+      <c r="C15" s="147" t="s">
+        <v>201</v>
+      </c>
+      <c r="D15" s="147" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="147" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="147">
+        <f>SUMIF($A$4:$A$12,A16,$D$4:$D$12)</f>
+        <v>100</v>
+      </c>
+      <c r="C16" s="147" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="147">
+        <v>100</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" ref="E16:E17" ca="1" si="1">_xlfn.FORMULATEXT(B16)</f>
+        <v>=SUMIF($A$4:$A$12;A16;$D$4:$D$12)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="147" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" s="147">
+        <f t="shared" ref="B17:B18" si="2">SUMIF($A$4:$A$12,A17,$D$4:$D$12)</f>
+        <v>300</v>
+      </c>
+      <c r="C17" s="147" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="147">
+        <v>300</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=SUMIF($A$4:$A$12;A17;$D$4:$D$12)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="147" t="s">
+        <v>214</v>
+      </c>
+      <c r="B18" s="147">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="C18" s="147" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="147">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="146"/>
+      <c r="B19" s="146"/>
+      <c r="C19" s="146"/>
+      <c r="D19" s="146"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="146"/>
+      <c r="B20" s="146"/>
+      <c r="C20" s="146"/>
+      <c r="D20" s="146"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="147" t="s">
+        <v>229</v>
+      </c>
+      <c r="B21" s="147" t="s">
+        <v>230</v>
+      </c>
+      <c r="C21" s="147" t="s">
+        <v>201</v>
+      </c>
+      <c r="D21" s="147" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="147" t="s">
+        <v>209</v>
+      </c>
+      <c r="B22" s="147">
+        <f>SUMIF($B$4:$B$12,A22,$D$4:$D$12)</f>
+        <v>300</v>
+      </c>
+      <c r="C22" s="147" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="147">
+        <v>300</v>
+      </c>
+      <c r="E22" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B22)</f>
+        <v>=SUMIF($B$4:$B$12;A22;$D$4:$D$12)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="147" t="s">
+        <v>210</v>
+      </c>
+      <c r="B23" s="147">
+        <f t="shared" ref="B23:B24" si="3">SUMIF($B$4:$B$12,A23,$D$4:$D$12)</f>
+        <v>200</v>
+      </c>
+      <c r="C23" s="147" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="147">
+        <v>200</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" ref="E23:E24" ca="1" si="4">_xlfn.FORMULATEXT(B23)</f>
+        <v>=SUMIF($B$4:$B$12;A23;$D$4:$D$12)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="147" t="s">
+        <v>211</v>
+      </c>
+      <c r="B24" s="147">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="C24" s="147" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="147">
+        <v>200</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>=SUMIF($B$4:$B$12;A24;$D$4:$D$12)</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{924B0E65-FB22-4426-BF98-A239FDE19170}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="20.399999999999999" thickBot="1">
+      <c r="A1" s="279" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="279"/>
+      <c r="C1" s="279"/>
+      <c r="D1" s="279"/>
+      <c r="E1" s="279"/>
+      <c r="F1" s="279"/>
+      <c r="G1" s="279"/>
+      <c r="H1" s="279"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickTop="1"/>
+    <row r="3" spans="1:10" ht="18" thickBot="1">
+      <c r="A3" s="280" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" s="280"/>
+      <c r="C3" s="280"/>
+      <c r="D3" s="280"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickTop="1">
+      <c r="A4" s="220"/>
+      <c r="B4" s="219" t="s">
+        <v>239</v>
+      </c>
+      <c r="C4" s="219" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" s="219" t="s">
+        <v>241</v>
+      </c>
+      <c r="E4" s="146" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="149" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" s="198">
+        <v>10</v>
+      </c>
+      <c r="C5" s="198">
+        <v>4</v>
+      </c>
+      <c r="D5" s="199">
+        <v>9</v>
+      </c>
+      <c r="E5" s="146">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="149" t="s">
+        <v>237</v>
+      </c>
+      <c r="B6" s="198">
+        <v>12</v>
+      </c>
+      <c r="C6" s="198">
+        <v>6</v>
+      </c>
+      <c r="D6" s="199">
+        <v>8</v>
+      </c>
+      <c r="E6" s="146">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1">
+      <c r="A7" s="149" t="s">
+        <v>238</v>
+      </c>
+      <c r="B7" s="221">
+        <v>8</v>
+      </c>
+      <c r="C7" s="221">
+        <v>9</v>
+      </c>
+      <c r="D7" s="222">
+        <v>5</v>
+      </c>
+      <c r="E7" s="146">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="146" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="146">
+        <v>50</v>
+      </c>
+      <c r="C8" s="146">
+        <v>40</v>
+      </c>
+      <c r="D8" s="146">
+        <v>60</v>
+      </c>
+      <c r="E8" s="146"/>
+      <c r="G8" s="281" t="s">
+        <v>221</v>
+      </c>
+      <c r="H8" s="217">
+        <f>SUMPRODUCT(B5:D7,B12:D14)</f>
+        <v>1060</v>
+      </c>
+      <c r="J8" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(H8)</f>
+        <v>=SUMPRODUCT(B5:D7;B12:D14)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18" thickBot="1">
+      <c r="A10" s="280" t="s">
+        <v>245</v>
+      </c>
+      <c r="B10" s="280"/>
+      <c r="C10" s="280"/>
+      <c r="D10" s="280"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.6" customHeight="1" thickTop="1">
+      <c r="A11" s="220"/>
+      <c r="B11" s="219" t="s">
+        <v>239</v>
+      </c>
+      <c r="C11" s="219" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" s="219" t="s">
+        <v>241</v>
+      </c>
+      <c r="E11" s="146" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="149" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" s="218">
+        <v>40</v>
+      </c>
+      <c r="C12" s="218">
+        <v>40</v>
+      </c>
+      <c r="D12" s="218">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <f>SUM(B12:D12)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="149" t="s">
+        <v>237</v>
+      </c>
+      <c r="B13" s="218">
+        <v>0</v>
+      </c>
+      <c r="C13" s="218">
+        <v>0</v>
+      </c>
+      <c r="D13" s="218">
+        <v>40</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" ref="E13:E14" si="0">SUM(B13:D13)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="149" t="s">
+        <v>238</v>
+      </c>
+      <c r="B14" s="218">
+        <v>10</v>
+      </c>
+      <c r="C14" s="218">
+        <v>0</v>
+      </c>
+      <c r="D14" s="218">
+        <v>20</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="146" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" s="146">
+        <f>SUM(B12:B14)</f>
+        <v>50</v>
+      </c>
+      <c r="C15" s="146">
+        <f t="shared" ref="C15:D15" si="1">SUM(C12:C14)</f>
+        <v>40</v>
+      </c>
+      <c r="D15" s="146">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
+  <phoneticPr fontId="16" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6609289-8039-4CB8-88EB-4CAB760EEE88}">
   <dimension ref="A1:F18"/>
@@ -3568,11 +4710,11 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1"/>
     <row r="2" spans="1:6" ht="15" thickBot="1">
-      <c r="A2" s="149" t="s">
+      <c r="A2" s="228" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="150"/>
-      <c r="C2" s="151"/>
+      <c r="B2" s="229"/>
+      <c r="C2" s="230"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="18" t="s">
@@ -3703,10 +4845,10 @@
       <c r="A17" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="144" t="s">
+      <c r="B17" s="223" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="145"/>
+      <c r="C17" s="224"/>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1">
       <c r="A18" s="12" t="s">
@@ -3750,16 +4892,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1">
-      <c r="B1" s="149" t="s">
+      <c r="B1" s="228" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="150"/>
-      <c r="D1" s="151"/>
-      <c r="F1" s="164" t="s">
+      <c r="C1" s="229"/>
+      <c r="D1" s="230"/>
+      <c r="F1" s="243" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="165"/>
-      <c r="H1" s="166"/>
+      <c r="G1" s="244"/>
+      <c r="H1" s="245"/>
     </row>
     <row r="2" spans="2:9">
       <c r="B2" s="68"/>
@@ -3810,11 +4952,11 @@
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1"/>
     <row r="6" spans="2:9" ht="15" thickBot="1">
-      <c r="B6" s="169" t="s">
+      <c r="B6" s="248" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="170"/>
-      <c r="D6" s="171"/>
+      <c r="C6" s="249"/>
+      <c r="D6" s="250"/>
       <c r="F6" s="1"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -3898,10 +5040,10 @@
       <c r="F11" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="167" t="s">
+      <c r="G11" s="246" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="168"/>
+      <c r="H11" s="247"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1">
       <c r="B12" s="63" t="s">
@@ -3958,15 +5100,15 @@
     </row>
     <row r="15" spans="2:9" ht="15" thickBot="1"/>
     <row r="16" spans="2:9" ht="15" thickBot="1">
-      <c r="B16" s="161" t="s">
+      <c r="B16" s="240" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="162"/>
-      <c r="D16" s="162"/>
-      <c r="E16" s="162"/>
-      <c r="F16" s="162"/>
-      <c r="G16" s="162"/>
-      <c r="H16" s="163"/>
+      <c r="C16" s="241"/>
+      <c r="D16" s="241"/>
+      <c r="E16" s="241"/>
+      <c r="F16" s="241"/>
+      <c r="G16" s="241"/>
+      <c r="H16" s="242"/>
     </row>
     <row r="17" spans="2:9">
       <c r="B17" s="56" t="s">
@@ -4157,11 +5299,11 @@
         <f ca="1">_xlfn.FORMULATEXT(C2)</f>
         <v>=SUMPRODUCT(J4:K4;E8:F8)</v>
       </c>
-      <c r="I2" s="172" t="s">
+      <c r="I2" s="251" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="173"/>
-      <c r="K2" s="174"/>
+      <c r="J2" s="252"/>
+      <c r="K2" s="253"/>
     </row>
     <row r="3" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="I3" s="79"/>
@@ -4219,10 +5361,10 @@
       <c r="I6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="167" t="s">
+      <c r="J6" s="246" t="s">
         <v>85</v>
       </c>
-      <c r="K6" s="168"/>
+      <c r="K6" s="247"/>
     </row>
     <row r="7" spans="1:11" ht="15" thickBot="1">
       <c r="D7" s="63" t="s">
@@ -4256,15 +5398,15 @@
     </row>
     <row r="9" spans="1:11" ht="15" thickBot="1"/>
     <row r="10" spans="1:11" ht="15" thickBot="1">
-      <c r="A10" s="161" t="s">
+      <c r="A10" s="240" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="162"/>
-      <c r="C10" s="162"/>
-      <c r="D10" s="162"/>
-      <c r="E10" s="162"/>
-      <c r="F10" s="162"/>
-      <c r="G10" s="163"/>
+      <c r="B10" s="241"/>
+      <c r="C10" s="241"/>
+      <c r="D10" s="241"/>
+      <c r="E10" s="241"/>
+      <c r="F10" s="241"/>
+      <c r="G10" s="242"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="56" t="s">
@@ -4389,14 +5531,14 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1"/>
     <row r="2" spans="1:14" ht="21.6" thickBot="1">
-      <c r="D2" s="175" t="s">
+      <c r="D2" s="254" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="177"/>
+      <c r="E2" s="255"/>
+      <c r="F2" s="255"/>
+      <c r="G2" s="255"/>
+      <c r="H2" s="255"/>
+      <c r="I2" s="256"/>
     </row>
     <row r="3" spans="1:14">
       <c r="D3" s="104"/>
@@ -4477,18 +5619,18 @@
         <f>SUMPRODUCT(E4:I4,E5:I5)</f>
         <v>20300</v>
       </c>
-      <c r="D7" s="175" t="s">
+      <c r="D7" s="254" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="176"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="176"/>
-      <c r="H7" s="176"/>
-      <c r="I7" s="176"/>
-      <c r="J7" s="176"/>
-      <c r="K7" s="176"/>
-      <c r="L7" s="176"/>
-      <c r="M7" s="177"/>
+      <c r="E7" s="255"/>
+      <c r="F7" s="255"/>
+      <c r="G7" s="255"/>
+      <c r="H7" s="255"/>
+      <c r="I7" s="255"/>
+      <c r="J7" s="255"/>
+      <c r="K7" s="255"/>
+      <c r="L7" s="255"/>
+      <c r="M7" s="256"/>
     </row>
     <row r="8" spans="1:14" ht="15.6" thickTop="1" thickBot="1">
       <c r="D8" s="98" t="s">
@@ -4594,7 +5736,7 @@
         <v>100000</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" ref="N10:N12" ca="1" si="0">_xlfn.FORMULATEXT(J10)</f>
+        <f ca="1">_xlfn.FORMULATEXT(J10)</f>
         <v>=SUMPRODUCT($E$4:$I$4;E10:I10)</v>
       </c>
     </row>
@@ -4632,7 +5774,7 @@
         <v>25000</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">_xlfn.FORMULATEXT(J11)</f>
         <v>=SUMPRODUCT($E$4:$I$4;E11:I11)</v>
       </c>
     </row>
@@ -4670,7 +5812,7 @@
         <v>250000</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">_xlfn.FORMULATEXT(J12)</f>
         <v>=SUMPRODUCT($E$4:$I$4;E12:I12)</v>
       </c>
     </row>
@@ -4679,12 +5821,12 @@
       <c r="E16" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="178" t="s">
+      <c r="F16" s="257" t="s">
         <v>103</v>
       </c>
-      <c r="G16" s="179"/>
-      <c r="H16" s="179"/>
-      <c r="I16" s="180"/>
+      <c r="G16" s="258"/>
+      <c r="H16" s="258"/>
+      <c r="I16" s="259"/>
     </row>
     <row r="17" spans="5:6" ht="15" thickBot="1">
       <c r="E17" s="112" t="s">
@@ -4726,13 +5868,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:8" ht="20.399999999999999" thickBot="1">
-      <c r="D1" s="181" t="s">
+      <c r="D1" s="260" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="182"/>
-      <c r="F1" s="182"/>
-      <c r="G1" s="182"/>
-      <c r="H1" s="183"/>
+      <c r="E1" s="261"/>
+      <c r="F1" s="261"/>
+      <c r="G1" s="261"/>
+      <c r="H1" s="262"/>
     </row>
     <row r="2" spans="4:8" ht="15" thickBot="1">
       <c r="D2" s="127" t="s">
@@ -4935,7 +6077,7 @@
         <v>6</v>
       </c>
       <c r="I18" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(F18)</f>
+        <f t="shared" ref="I18:I23" ca="1" si="0">_xlfn.FORMULATEXT(F18)</f>
         <v>=SUM(E9:G9)</v>
       </c>
     </row>
@@ -4958,7 +6100,7 @@
         <v>5</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" ref="I19:I23" ca="1" si="0">_xlfn.FORMULATEXT(F19)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>=SUMPRODUCT(E3:G3;$E$9:$G$9)</v>
       </c>
     </row>
@@ -5059,10 +6201,10 @@
       <c r="E26" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="184" t="s">
+      <c r="F26" s="263" t="s">
         <v>135</v>
       </c>
-      <c r="G26" s="185"/>
+      <c r="G26" s="264"/>
     </row>
     <row r="27" spans="4:9" ht="15" thickBot="1">
       <c r="E27" s="143" t="s">
@@ -5110,229 +6252,227 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:14" ht="20.399999999999999" thickBot="1">
-      <c r="J1" s="231" t="s">
+      <c r="J1" s="267" t="s">
         <v>170</v>
       </c>
-      <c r="K1" s="232"/>
-      <c r="L1" s="232"/>
-      <c r="M1" s="233"/>
+      <c r="K1" s="268"/>
+      <c r="L1" s="268"/>
+      <c r="M1" s="269"/>
     </row>
     <row r="2" spans="3:14" ht="15" thickBot="1">
-      <c r="D2" s="221" t="s">
+      <c r="D2" s="177" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="222" t="s">
+      <c r="E2" s="178" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="222" t="s">
+      <c r="F2" s="178" t="s">
         <v>137</v>
       </c>
-      <c r="G2" s="222" t="s">
+      <c r="G2" s="178" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="223" t="s">
+      <c r="H2" s="179" t="s">
         <v>139</v>
       </c>
-      <c r="J2" s="227"/>
-      <c r="K2" s="228" t="s">
+      <c r="J2" s="183"/>
+      <c r="K2" s="184" t="s">
         <v>143</v>
       </c>
-      <c r="L2" s="229" t="s">
+      <c r="L2" s="185" t="s">
         <v>144</v>
       </c>
-      <c r="M2" s="230" t="s">
+      <c r="M2" s="186" t="s">
         <v>145</v>
       </c>
-      <c r="N2" s="188"/>
+      <c r="N2" s="146"/>
     </row>
     <row r="3" spans="3:14">
-      <c r="D3" s="224" t="s">
+      <c r="D3" s="180" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="209">
+      <c r="E3" s="167">
         <v>700</v>
       </c>
-      <c r="F3" s="207">
+      <c r="F3" s="165">
         <v>5</v>
       </c>
-      <c r="G3" s="207">
+      <c r="G3" s="165">
         <v>8</v>
       </c>
-      <c r="H3" s="208">
+      <c r="H3" s="166">
         <v>6</v>
       </c>
-      <c r="J3" s="201" t="s">
+      <c r="J3" s="159" t="s">
         <v>110</v>
       </c>
-      <c r="K3" s="198">
+      <c r="K3" s="156">
         <v>400</v>
       </c>
-      <c r="L3" s="196">
+      <c r="L3" s="154">
         <v>0</v>
       </c>
-      <c r="M3" s="197">
+      <c r="M3" s="155">
         <v>300</v>
       </c>
-      <c r="N3" s="188"/>
+      <c r="N3" s="146"/>
     </row>
     <row r="4" spans="3:14">
-      <c r="D4" s="225" t="s">
+      <c r="D4" s="181" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="210">
+      <c r="E4" s="168">
         <v>500</v>
       </c>
-      <c r="F4" s="186">
+      <c r="F4" s="144">
         <v>0</v>
       </c>
-      <c r="G4" s="186">
+      <c r="G4" s="144">
         <v>4</v>
       </c>
-      <c r="H4" s="204">
+      <c r="H4" s="162">
         <v>12</v>
       </c>
-      <c r="J4" s="202" t="s">
+      <c r="J4" s="160" t="s">
         <v>111</v>
       </c>
-      <c r="K4" s="199">
+      <c r="K4" s="157">
         <v>500</v>
       </c>
-      <c r="L4" s="190">
+      <c r="L4" s="148">
         <v>0</v>
       </c>
-      <c r="M4" s="192">
+      <c r="M4" s="150">
         <v>0</v>
       </c>
-      <c r="N4" s="188"/>
+      <c r="N4" s="146"/>
     </row>
     <row r="5" spans="3:14">
-      <c r="D5" s="225" t="s">
+      <c r="D5" s="181" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="210">
+      <c r="E5" s="168">
         <v>100</v>
       </c>
-      <c r="F5" s="186">
+      <c r="F5" s="144">
         <v>4</v>
       </c>
-      <c r="G5" s="186">
+      <c r="G5" s="144">
         <v>0</v>
       </c>
-      <c r="H5" s="204">
+      <c r="H5" s="162">
         <v>7</v>
       </c>
-      <c r="J5" s="202" t="s">
+      <c r="J5" s="160" t="s">
         <v>112</v>
       </c>
-      <c r="K5" s="199">
+      <c r="K5" s="157">
         <v>0</v>
       </c>
-      <c r="L5" s="190">
+      <c r="L5" s="148">
         <v>100</v>
       </c>
-      <c r="M5" s="192">
+      <c r="M5" s="150">
         <v>0</v>
       </c>
-      <c r="N5" s="188"/>
+      <c r="N5" s="146"/>
     </row>
     <row r="6" spans="3:14">
-      <c r="D6" s="225" t="s">
+      <c r="D6" s="181" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="210">
+      <c r="E6" s="168">
         <v>800</v>
       </c>
-      <c r="F6" s="186">
+      <c r="F6" s="144">
         <v>7</v>
       </c>
-      <c r="G6" s="186">
+      <c r="G6" s="144">
         <v>2</v>
       </c>
-      <c r="H6" s="204">
+      <c r="H6" s="162">
         <v>5</v>
       </c>
-      <c r="J6" s="202" t="s">
+      <c r="J6" s="160" t="s">
         <v>113</v>
       </c>
-      <c r="K6" s="199">
+      <c r="K6" s="157">
         <v>0</v>
       </c>
-      <c r="L6" s="190">
+      <c r="L6" s="148">
         <v>800</v>
       </c>
-      <c r="M6" s="192">
+      <c r="M6" s="150">
         <v>0</v>
       </c>
-      <c r="N6" s="188"/>
+      <c r="N6" s="146"/>
     </row>
     <row r="7" spans="3:14" ht="15" thickBot="1">
-      <c r="D7" s="226" t="s">
+      <c r="D7" s="182" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="211">
+      <c r="E7" s="169">
         <v>400</v>
       </c>
-      <c r="F7" s="205">
+      <c r="F7" s="163">
         <v>12</v>
       </c>
-      <c r="G7" s="205">
+      <c r="G7" s="163">
         <v>7</v>
       </c>
-      <c r="H7" s="206">
+      <c r="H7" s="164">
         <v>0</v>
       </c>
-      <c r="J7" s="202" t="s">
+      <c r="J7" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="K7" s="199">
+      <c r="K7" s="157">
         <v>0</v>
       </c>
-      <c r="L7" s="190">
+      <c r="L7" s="148">
         <v>0</v>
       </c>
-      <c r="M7" s="192">
+      <c r="M7" s="150">
         <v>400</v>
       </c>
-      <c r="N7" s="188"/>
+      <c r="N7" s="146"/>
     </row>
     <row r="8" spans="3:14" ht="15" thickBot="1">
-      <c r="D8" s="187"/>
-      <c r="J8" s="203" t="s">
+      <c r="D8" s="145"/>
+      <c r="J8" s="161" t="s">
         <v>153</v>
       </c>
-      <c r="K8" s="200">
+      <c r="K8" s="158">
         <f>SUMPRODUCT(K3:K7,F3:F7)</f>
         <v>2000</v>
       </c>
-      <c r="L8" s="194">
+      <c r="L8" s="152">
         <f>SUMPRODUCT(L3:L7,G3:G7)</f>
         <v>1600</v>
       </c>
       <c r="M8" s="55">
-        <f t="shared" ref="L8:M8" si="0">SUMPRODUCT(M3:M7,H3:H7)</f>
+        <f>SUMPRODUCT(M3:M7,H3:H7)</f>
         <v>1800</v>
       </c>
-      <c r="N8" s="188" t="s">
+      <c r="N8" s="146" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="3:14" ht="15" thickBot="1">
-      <c r="D9" s="240"/>
-    </row>
+    <row r="9" spans="3:14" ht="15" thickBot="1"/>
     <row r="10" spans="3:14" ht="15" thickBot="1">
-      <c r="E10" s="234" t="s">
+      <c r="E10" s="187" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="235" t="s">
+      <c r="F10" s="188" t="s">
         <v>141</v>
       </c>
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="3:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="E11" s="236" t="s">
+      <c r="E11" s="189" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="237">
+      <c r="F11" s="190">
         <f>SUM(K8:M8)</f>
         <v>5400</v>
       </c>
@@ -5342,10 +6482,10 @@
       </c>
     </row>
     <row r="12" spans="3:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="E12" s="238" t="s">
+      <c r="E12" s="191" t="s">
         <v>142</v>
       </c>
-      <c r="F12" s="239">
+      <c r="F12" s="192">
         <v>900</v>
       </c>
       <c r="G12" s="8" t="s">
@@ -5354,37 +6494,37 @@
     </row>
     <row r="13" spans="3:14" ht="15" thickBot="1"/>
     <row r="14" spans="3:14" ht="15" thickBot="1">
-      <c r="C14" s="221" t="s">
+      <c r="C14" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="222" t="s">
+      <c r="D14" s="178" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="222" t="s">
+      <c r="E14" s="178" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="222" t="s">
+      <c r="F14" s="178" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="223" t="s">
+      <c r="G14" s="179" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="3:14">
-      <c r="C15" s="195" t="s">
+      <c r="C15" s="153" t="s">
         <v>150</v>
       </c>
-      <c r="D15" s="213" t="s">
+      <c r="D15" s="171" t="s">
         <v>146</v>
       </c>
-      <c r="E15" s="213">
+      <c r="E15" s="171">
         <f>SUM(K3:K7)</f>
         <v>900</v>
       </c>
-      <c r="F15" s="213" t="s">
+      <c r="F15" s="171" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="214">
+      <c r="G15" s="172">
         <f>$F$12</f>
         <v>900</v>
       </c>
@@ -5394,185 +6534,185 @@
       </c>
     </row>
     <row r="16" spans="3:14">
-      <c r="C16" s="191" t="s">
+      <c r="C16" s="149" t="s">
         <v>151</v>
       </c>
-      <c r="D16" s="189" t="s">
+      <c r="D16" s="147" t="s">
         <v>147</v>
       </c>
-      <c r="E16" s="189">
+      <c r="E16" s="147">
         <f>SUM(L3:L7)</f>
         <v>900</v>
       </c>
-      <c r="F16" s="189" t="s">
+      <c r="F16" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="212">
+      <c r="G16" s="170">
         <f>$F$12</f>
         <v>900</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" ref="H16:H22" ca="1" si="1">_xlfn.FORMULATEXT(E16)</f>
+        <f t="shared" ref="H16:H22" ca="1" si="0">_xlfn.FORMULATEXT(E16)</f>
         <v>=SUM(L3:L7)</v>
       </c>
     </row>
     <row r="17" spans="3:8">
-      <c r="C17" s="191" t="s">
+      <c r="C17" s="149" t="s">
         <v>152</v>
       </c>
-      <c r="D17" s="189" t="s">
+      <c r="D17" s="147" t="s">
         <v>148</v>
       </c>
-      <c r="E17" s="189">
+      <c r="E17" s="147">
         <f>SUM(M3:M7)</f>
         <v>700</v>
       </c>
-      <c r="F17" s="189" t="s">
+      <c r="F17" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="212">
+      <c r="G17" s="170">
         <f>$F$12</f>
         <v>900</v>
       </c>
       <c r="H17" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>=SUM(M3:M7)</v>
       </c>
     </row>
     <row r="18" spans="3:8">
-      <c r="C18" s="191" t="s">
+      <c r="C18" s="149" t="s">
         <v>154</v>
       </c>
-      <c r="D18" s="189" t="s">
+      <c r="D18" s="147" t="s">
         <v>159</v>
       </c>
-      <c r="E18" s="189">
+      <c r="E18" s="147">
         <f>SUM(K3:M3)</f>
         <v>700</v>
       </c>
-      <c r="F18" s="189" t="s">
+      <c r="F18" s="147" t="s">
         <v>149</v>
       </c>
-      <c r="G18" s="212">
+      <c r="G18" s="170">
         <f>E3</f>
         <v>700</v>
       </c>
       <c r="H18" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>=SUM(K3:M3)</v>
       </c>
     </row>
     <row r="19" spans="3:8">
-      <c r="C19" s="191" t="s">
+      <c r="C19" s="149" t="s">
         <v>155</v>
       </c>
-      <c r="D19" s="189" t="s">
+      <c r="D19" s="147" t="s">
         <v>160</v>
       </c>
-      <c r="E19" s="189">
-        <f t="shared" ref="E19:E22" si="2">SUM(K4:M4)</f>
+      <c r="E19" s="147">
+        <f>SUM(K4:M4)</f>
         <v>500</v>
       </c>
-      <c r="F19" s="189" t="s">
+      <c r="F19" s="147" t="s">
         <v>149</v>
       </c>
-      <c r="G19" s="212">
-        <f t="shared" ref="G19:G22" si="3">E4</f>
+      <c r="G19" s="170">
+        <f>E4</f>
         <v>500</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>=SUM(K4:M4)</v>
       </c>
     </row>
     <row r="20" spans="3:8">
-      <c r="C20" s="191" t="s">
+      <c r="C20" s="149" t="s">
         <v>156</v>
       </c>
-      <c r="D20" s="189" t="s">
+      <c r="D20" s="147" t="s">
         <v>161</v>
       </c>
-      <c r="E20" s="189">
-        <f t="shared" si="2"/>
+      <c r="E20" s="147">
+        <f>SUM(K5:M5)</f>
         <v>100</v>
       </c>
-      <c r="F20" s="189" t="s">
+      <c r="F20" s="147" t="s">
         <v>149</v>
       </c>
-      <c r="G20" s="212">
-        <f t="shared" si="3"/>
+      <c r="G20" s="170">
+        <f>E5</f>
         <v>100</v>
       </c>
       <c r="H20" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>=SUM(K5:M5)</v>
       </c>
     </row>
     <row r="21" spans="3:8">
-      <c r="C21" s="191" t="s">
+      <c r="C21" s="149" t="s">
         <v>157</v>
       </c>
-      <c r="D21" s="189" t="s">
+      <c r="D21" s="147" t="s">
         <v>162</v>
       </c>
-      <c r="E21" s="189">
-        <f t="shared" si="2"/>
+      <c r="E21" s="147">
+        <f>SUM(K6:M6)</f>
         <v>800</v>
       </c>
-      <c r="F21" s="189" t="s">
+      <c r="F21" s="147" t="s">
         <v>149</v>
       </c>
-      <c r="G21" s="212">
-        <f t="shared" si="3"/>
+      <c r="G21" s="170">
+        <f>E6</f>
         <v>800</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>=SUM(K6:M6)</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="15" thickBot="1">
-      <c r="C22" s="193" t="s">
+      <c r="C22" s="151" t="s">
         <v>158</v>
       </c>
-      <c r="D22" s="194" t="s">
+      <c r="D22" s="152" t="s">
         <v>163</v>
       </c>
-      <c r="E22" s="194">
-        <f t="shared" si="2"/>
+      <c r="E22" s="152">
+        <f>SUM(K7:M7)</f>
         <v>400</v>
       </c>
-      <c r="F22" s="194" t="s">
+      <c r="F22" s="152" t="s">
         <v>149</v>
       </c>
       <c r="G22" s="55">
-        <f t="shared" si="3"/>
+        <f>E7</f>
         <v>400</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>=SUM(K7:M7)</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="15" thickBot="1"/>
     <row r="25" spans="3:8" ht="29.4" thickBot="1">
-      <c r="D25" s="215" t="s">
+      <c r="D25" s="173" t="s">
         <v>168</v>
       </c>
-      <c r="E25" s="216" t="s">
+      <c r="E25" s="265" t="s">
         <v>169</v>
       </c>
-      <c r="F25" s="217"/>
+      <c r="F25" s="266"/>
     </row>
     <row r="26" spans="3:8" ht="29.4" thickBot="1">
-      <c r="D26" s="218" t="s">
+      <c r="D26" s="174" t="s">
         <v>166</v>
       </c>
-      <c r="E26" s="219">
+      <c r="E26" s="175">
         <f>F11</f>
         <v>5400</v>
       </c>
-      <c r="F26" s="220" t="s">
+      <c r="F26" s="176" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5589,7 +6729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681C5319-DF78-4C4C-8C5A-7F8DAFBD55C4}">
   <dimension ref="D1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -5606,131 +6746,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:15">
-      <c r="D1" s="189" t="s">
+      <c r="D1" s="147" t="s">
         <v>171</v>
       </c>
-      <c r="E1" s="189" t="s">
+      <c r="E1" s="147" t="s">
         <v>175</v>
       </c>
-      <c r="F1" s="189" t="s">
+      <c r="F1" s="147" t="s">
         <v>181</v>
       </c>
-      <c r="G1" s="189" t="s">
+      <c r="G1" s="147" t="s">
         <v>180</v>
       </c>
-      <c r="H1" s="189" t="s">
+      <c r="H1" s="147" t="s">
         <v>179</v>
       </c>
-      <c r="I1" s="189" t="s">
+      <c r="I1" s="147" t="s">
         <v>176</v>
       </c>
       <c r="K1" s="6"/>
-      <c r="L1" s="189" t="s">
+      <c r="L1" s="147" t="s">
         <v>172</v>
       </c>
-      <c r="M1" s="189" t="s">
+      <c r="M1" s="147" t="s">
         <v>173</v>
       </c>
-      <c r="N1" s="189" t="s">
+      <c r="N1" s="147" t="s">
         <v>174</v>
       </c>
-      <c r="O1" s="241"/>
+      <c r="O1" s="146"/>
     </row>
     <row r="2" spans="4:15">
-      <c r="D2" s="189">
+      <c r="D2" s="147">
         <v>1</v>
       </c>
-      <c r="E2" s="242">
+      <c r="E2" s="193">
         <v>60</v>
       </c>
-      <c r="F2" s="189">
+      <c r="F2" s="147">
         <v>50</v>
       </c>
-      <c r="G2" s="190">
+      <c r="G2" s="148">
         <f>IF($E2&gt;$F2,ABS($E2-$F2),0)</f>
         <v>10</v>
       </c>
-      <c r="H2" s="190">
+      <c r="H2" s="148">
         <f>IF($E2&lt;$F2,ABS($E2-$F2),0)</f>
         <v>0</v>
       </c>
-      <c r="I2" s="189">
-        <f>F2+G2-H2</f>
+      <c r="I2" s="147">
+        <f t="shared" ref="I2:I7" si="0">F2+G2-H2</f>
         <v>60</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="189">
+      <c r="L2" s="147">
         <v>10000</v>
       </c>
-      <c r="M2" s="189">
+      <c r="M2" s="147">
         <v>2000</v>
       </c>
-      <c r="N2" s="189">
+      <c r="N2" s="147">
         <v>4000</v>
       </c>
     </row>
     <row r="3" spans="4:15">
-      <c r="D3" s="189">
+      <c r="D3" s="147">
         <v>2</v>
       </c>
-      <c r="E3" s="242">
+      <c r="E3" s="193">
         <v>70</v>
       </c>
-      <c r="F3" s="189">
+      <c r="F3" s="147">
         <f>I2</f>
         <v>60</v>
       </c>
-      <c r="G3" s="190">
-        <f t="shared" ref="G3:G6" si="0">IF($E3&gt;$F3,ABS($E3-$F3),0)</f>
+      <c r="G3" s="148">
+        <f>IF($E3&gt;$F3,ABS($E3-$F3),0)</f>
         <v>10</v>
       </c>
-      <c r="H3" s="190">
-        <f t="shared" ref="H3:H6" si="1">IF($E3&lt;$F3,ABS($E3-$F3),0)</f>
+      <c r="H3" s="148">
+        <f>IF($E3&lt;$F3,ABS($E3-$F3),0)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="189">
-        <f>F3+G3-H3</f>
+      <c r="I3" s="147">
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="L3" s="246">
+      <c r="L3" s="6">
         <f>E7</f>
         <v>320</v>
       </c>
-      <c r="M3" s="246">
+      <c r="M3" s="6">
         <f>H7</f>
         <v>20</v>
       </c>
-      <c r="N3" s="246">
+      <c r="N3" s="6">
         <f>G7</f>
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="4:15">
-      <c r="D4" s="189">
+      <c r="D4" s="147">
         <v>3</v>
       </c>
-      <c r="E4" s="242">
+      <c r="E4" s="193">
         <v>50</v>
       </c>
-      <c r="F4" s="189">
+      <c r="F4" s="147">
         <f>I3</f>
         <v>70</v>
       </c>
-      <c r="G4" s="190">
+      <c r="G4" s="148">
+        <f>IF($E4&gt;$F4,ABS($E4-$F4),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="148">
+        <f>IF($E4&lt;$F4,ABS($E4-$F4),0)</f>
+        <v>20</v>
+      </c>
+      <c r="I4" s="147">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H4" s="190">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="I4" s="189">
-        <f>F4+G4-H4</f>
         <v>50</v>
       </c>
       <c r="K4" s="6" t="s">
@@ -5741,65 +6881,65 @@
         <v>3200000</v>
       </c>
       <c r="M4" s="38">
-        <f t="shared" ref="M4:N4" si="2">PRODUCT(M2:M3)</f>
+        <f>PRODUCT(M2:M3)</f>
         <v>40000</v>
       </c>
       <c r="N4" s="38">
-        <f t="shared" si="2"/>
+        <f>PRODUCT(N2:N3)</f>
         <v>180000</v>
       </c>
     </row>
     <row r="5" spans="4:15" ht="15" thickBot="1">
-      <c r="D5" s="189">
+      <c r="D5" s="147">
         <v>4</v>
       </c>
-      <c r="E5" s="242">
+      <c r="E5" s="193">
         <v>65</v>
       </c>
-      <c r="F5" s="189">
+      <c r="F5" s="147">
         <f>I4</f>
         <v>50</v>
       </c>
-      <c r="G5" s="190">
+      <c r="G5" s="148">
+        <f>IF($E5&gt;$F5,ABS($E5-$F5),0)</f>
+        <v>15</v>
+      </c>
+      <c r="H5" s="148">
+        <f>IF($E5&lt;$F5,ABS($E5-$F5),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="147">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="H5" s="190">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="189">
-        <f>F5+G5-H5</f>
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="4:15" ht="15.6" thickTop="1" thickBot="1">
-      <c r="D6" s="189">
+      <c r="D6" s="147">
         <v>5</v>
       </c>
-      <c r="E6" s="242">
+      <c r="E6" s="193">
         <v>75</v>
       </c>
-      <c r="F6" s="189">
+      <c r="F6" s="147">
         <f>I5</f>
         <v>65</v>
       </c>
-      <c r="G6" s="190">
+      <c r="G6" s="148">
+        <f>IF($E6&gt;$F6,ABS($E6-$F6),0)</f>
+        <v>10</v>
+      </c>
+      <c r="H6" s="148">
+        <f>IF($E6&lt;$F6,ABS($E6-$F6),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="147">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H6" s="190">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="189">
-        <f>F6+G6-H6</f>
         <v>75</v>
       </c>
       <c r="M6" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="244">
+      <c r="N6" s="195">
         <f>SUM(L4:N4)</f>
         <v>3420000</v>
       </c>
@@ -5808,24 +6948,24 @@
       <c r="D7" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="E7" s="245">
+      <c r="E7" s="196">
         <f>SUM(E2:E6)</f>
         <v>320</v>
       </c>
-      <c r="F7" s="189">
+      <c r="F7" s="147">
         <f>SUM(F2:F6)</f>
         <v>295</v>
       </c>
-      <c r="G7" s="189">
+      <c r="G7" s="147">
         <f>SUM(G2:G6)</f>
         <v>45</v>
       </c>
-      <c r="H7" s="189">
+      <c r="H7" s="147">
         <f>SUM(H2:H6)</f>
         <v>20</v>
       </c>
-      <c r="I7" s="189">
-        <f>F7+G7-H7</f>
+      <c r="I7" s="147">
+        <f t="shared" si="0"/>
         <v>320</v>
       </c>
       <c r="M7" t="s">
@@ -5836,7 +6976,7 @@
       </c>
     </row>
     <row r="9" spans="4:15">
-      <c r="G9" s="243"/>
+      <c r="G9" s="194"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5847,8 +6987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CB8FE9-35E3-45FA-8884-F9DB9B5AB336}">
   <dimension ref="D1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5863,42 +7003,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:13" ht="20.399999999999999" thickBot="1">
-      <c r="E1" s="231" t="s">
+      <c r="E1" s="267" t="s">
         <v>203</v>
       </c>
-      <c r="F1" s="232"/>
-      <c r="G1" s="233"/>
-      <c r="I1" s="256" t="s">
+      <c r="F1" s="268"/>
+      <c r="G1" s="269"/>
+      <c r="I1" s="270" t="s">
         <v>190</v>
       </c>
-      <c r="J1" s="257"/>
+      <c r="J1" s="271"/>
     </row>
     <row r="2" spans="4:13">
-      <c r="E2" s="195"/>
-      <c r="F2" s="252" t="s">
+      <c r="E2" s="153"/>
+      <c r="F2" s="202" t="s">
         <v>191</v>
       </c>
-      <c r="G2" s="253" t="s">
+      <c r="G2" s="203" t="s">
         <v>193</v>
       </c>
-      <c r="I2" s="258" t="s">
+      <c r="I2" s="206" t="s">
         <v>188</v>
       </c>
-      <c r="J2" s="259" t="s">
+      <c r="J2" s="207" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="3" spans="4:13" ht="15" thickBot="1">
-      <c r="E3" s="254" t="s">
+      <c r="E3" s="204" t="s">
         <v>185</v>
       </c>
-      <c r="F3" s="189">
+      <c r="F3" s="147">
         <v>1.5</v>
       </c>
-      <c r="G3" s="212">
+      <c r="G3" s="170">
         <v>3</v>
       </c>
-      <c r="I3" s="193">
+      <c r="I3" s="151">
         <v>42</v>
       </c>
       <c r="J3" s="55">
@@ -5906,35 +7046,35 @@
       </c>
     </row>
     <row r="4" spans="4:13">
-      <c r="E4" s="254" t="s">
+      <c r="E4" s="204" t="s">
         <v>186</v>
       </c>
-      <c r="F4" s="189">
+      <c r="F4" s="147">
         <v>3</v>
       </c>
-      <c r="G4" s="212">
+      <c r="G4" s="170">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="4:13">
-      <c r="E5" s="254" t="s">
+      <c r="E5" s="204" t="s">
         <v>192</v>
       </c>
-      <c r="F5" s="248">
+      <c r="F5" s="198">
         <v>20</v>
       </c>
-      <c r="G5" s="249">
+      <c r="G5" s="199">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="4:13" ht="15" thickBot="1">
-      <c r="E6" s="255" t="s">
+      <c r="E6" s="205" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="250">
+      <c r="F6" s="200">
         <v>4</v>
       </c>
-      <c r="G6" s="251">
+      <c r="G6" s="201">
         <v>12</v>
       </c>
       <c r="I6" s="60" t="s">
@@ -5945,10 +7085,10 @@
       </c>
     </row>
     <row r="7" spans="4:13" ht="15.6" thickTop="1" thickBot="1">
-      <c r="I7" s="262" t="s">
+      <c r="I7" s="210" t="s">
         <v>197</v>
       </c>
-      <c r="J7" s="261">
+      <c r="J7" s="209">
         <f>SUMPRODUCT(F6:G6,F5:G5)</f>
         <v>200</v>
       </c>
@@ -5957,76 +7097,76 @@
     </row>
     <row r="8" spans="4:13" ht="15" thickTop="1"/>
     <row r="10" spans="4:13">
-      <c r="D10" s="247" t="s">
+      <c r="D10" s="197" t="s">
         <v>198</v>
       </c>
-      <c r="E10" s="247" t="s">
+      <c r="E10" s="197" t="s">
         <v>199</v>
       </c>
-      <c r="F10" s="247" t="s">
+      <c r="F10" s="197" t="s">
         <v>200</v>
       </c>
-      <c r="G10" s="247" t="s">
+      <c r="G10" s="197" t="s">
         <v>201</v>
       </c>
-      <c r="H10" s="247" t="s">
+      <c r="H10" s="197" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="11" spans="4:13">
-      <c r="D11" s="260" t="s">
+      <c r="D11" s="208" t="s">
         <v>194</v>
       </c>
-      <c r="E11" s="189" t="s">
+      <c r="E11" s="147" t="s">
         <v>187</v>
       </c>
-      <c r="F11" s="189">
+      <c r="F11" s="147">
         <f>SUMPRODUCT(F3:G3,F6:G6)</f>
         <v>42</v>
       </c>
-      <c r="G11" s="189" t="s">
+      <c r="G11" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="189">
+      <c r="H11" s="147">
         <f>I3</f>
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="4:13">
-      <c r="D12" s="260" t="s">
+      <c r="D12" s="208" t="s">
         <v>195</v>
       </c>
-      <c r="E12" s="189" t="s">
+      <c r="E12" s="147" t="s">
         <v>196</v>
       </c>
-      <c r="F12" s="189">
+      <c r="F12" s="147">
         <f>SUMPRODUCT(F6:G6,F4:G4)</f>
         <v>24</v>
       </c>
-      <c r="G12" s="189" t="s">
+      <c r="G12" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="189">
+      <c r="H12" s="147">
         <f>J3</f>
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="4:13" ht="15" thickBot="1"/>
     <row r="14" spans="4:13" ht="15" customHeight="1" thickBot="1">
-      <c r="E14" s="215" t="s">
+      <c r="E14" s="173" t="s">
         <v>205</v>
       </c>
-      <c r="F14" s="264" t="s">
+      <c r="F14" s="272" t="s">
         <v>206</v>
       </c>
-      <c r="G14" s="265"/>
-      <c r="H14" s="266"/>
+      <c r="G14" s="273"/>
+      <c r="H14" s="274"/>
     </row>
     <row r="15" spans="4:13" ht="15" thickBot="1">
-      <c r="E15" s="218" t="s">
+      <c r="E15" s="174" t="s">
         <v>207</v>
       </c>
-      <c r="F15" s="263">
+      <c r="F15" s="211">
         <f>J7</f>
         <v>200</v>
       </c>

</xml_diff>